<commit_message>
trial run of biogenic_refinery
</commit_message>
<xml_diff>
--- a/dmsan/biogenic_refinery/scores/China/parameters.xlsx
+++ b/dmsan/biogenic_refinery/scores/China/parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="BiogenicRefinery A" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="BiogenicRefinery B" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BiogenicRefinery A" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BiogenicRefinery B" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -477,7 +477,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>('Oil heat exchanger-A10', 'Orc cost [USD]')</t>
+          <t>('Oil heat exchanger-A10', 'Oil heat exchanger orc cost [USD]')</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
@@ -493,7 +493,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>('Oil heat exchanger-A10', 'Oil pump power [kW]')</t>
+          <t>('Oil heat exchanger-A10', 'Oil heat exchanger oil pump power [kW]')</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
@@ -509,7 +509,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>('Oil heat exchanger-A10', 'Oil electrical energy generated [kW]')</t>
+          <t>('Oil heat exchanger-A10', 'Oil heat exchanger oil electrical energy generated [kW]')</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
@@ -525,7 +525,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>('Oil heat exchanger-A10', 'Oil flowrate [L/min]')</t>
+          <t>('Oil heat exchanger-A10', 'Oil heat exchanger oil flowrate [L/min]')</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
@@ -541,7 +541,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>('Oil heat exchanger-A10', 'Ohx temp [C]')</t>
+          <t>('Oil heat exchanger-A10', 'Oil heat exchanger ohx temp [C]')</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
@@ -557,7 +557,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>('Oil heat exchanger-A10', 'Oil temp in [C]')</t>
+          <t>('Oil heat exchanger-A10', 'Oil heat exchanger oil temp in [C]')</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
@@ -573,7 +573,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>('Oil heat exchanger-A10', 'Oil temp out [C]')</t>
+          <t>('Oil heat exchanger-A10', 'Oil heat exchanger oil temp out [C]')</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
@@ -589,7 +589,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>('Oil heat exchanger-A10', 'Amb temp [C]')</t>
+          <t>('Oil heat exchanger-A10', 'Oil heat exchanger amb temp [C]')</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
@@ -605,7 +605,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-A11', 'Heat exchanger hydronic steel [kg]')</t>
+          <t>('Hydronic heat exchanger-A11', 'Hydronic heat exchanger heat exchanger hydronic steel [kg]')</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
@@ -621,7 +621,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-A11', 'Heat exchanger hydronic stainless [kg]')</t>
+          <t>('Hydronic heat exchanger-A11', 'Hydronic heat exchanger heat exchanger hydronic stainless [kg]')</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
@@ -637,7 +637,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-A11', 'Water pump power [kW]')</t>
+          <t>('Hydronic heat exchanger-A11', 'Hydronic heat exchanger water pump power [kW]')</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
@@ -653,7 +653,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-A11', 'Hhx inducer fan power [kW]')</t>
+          <t>('Hydronic heat exchanger-A11', 'Hydronic heat exchanger hhx inducer fan power [kW]')</t>
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
@@ -669,7 +669,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-A11', 'Hhx stack [USD]')</t>
+          <t>('Hydronic heat exchanger-A11', 'Hydronic heat exchanger hhx stack [USD]')</t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
@@ -685,7 +685,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-A11', 'Hhx stack thermocouple [USD]')</t>
+          <t>('Hydronic heat exchanger-A11', 'Hydronic heat exchanger hhx stack thermocouple [USD]')</t>
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
@@ -701,7 +701,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-A11', 'Hhx oxygen sensor [USD]')</t>
+          <t>('Hydronic heat exchanger-A11', 'Hydronic heat exchanger hhx oxygen sensor [USD]')</t>
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
@@ -717,7 +717,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-A11', 'Hhx inducer fan [USD]')</t>
+          <t>('Hydronic heat exchanger-A11', 'Hydronic heat exchanger hhx inducer fan [USD]')</t>
         </is>
       </c>
       <c r="C17" t="inlineStr"/>
@@ -733,7 +733,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-A11', 'Hhx flow meter [USD]')</t>
+          <t>('Hydronic heat exchanger-A11', 'Hydronic heat exchanger hhx flow meter [USD]')</t>
         </is>
       </c>
       <c r="C18" t="inlineStr"/>
@@ -749,7 +749,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-A11', 'Hhx pump [USD]')</t>
+          <t>('Hydronic heat exchanger-A11', 'Hydronic heat exchanger hhx pump [USD]')</t>
         </is>
       </c>
       <c r="C19" t="inlineStr"/>
@@ -765,7 +765,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-A11', 'Hhx water in thermistor [USD]')</t>
+          <t>('Hydronic heat exchanger-A11', 'Hydronic heat exchanger hhx water in thermistor [USD]')</t>
         </is>
       </c>
       <c r="C20" t="inlineStr"/>
@@ -781,7 +781,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-A11', 'Hhx water out thermistor [USD]')</t>
+          <t>('Hydronic heat exchanger-A11', 'Hydronic heat exchanger hhx water out thermistor [USD]')</t>
         </is>
       </c>
       <c r="C21" t="inlineStr"/>
@@ -797,7 +797,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-A11', 'Hhx load tank [USD]')</t>
+          <t>('Hydronic heat exchanger-A11', 'Hydronic heat exchanger hhx load tank [USD]')</t>
         </is>
       </c>
       <c r="C22" t="inlineStr"/>
@@ -813,7 +813,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-A11', 'Hhx expansion tank [USD]')</t>
+          <t>('Hydronic heat exchanger-A11', 'Hydronic heat exchanger hhx expansion tank [USD]')</t>
         </is>
       </c>
       <c r="C23" t="inlineStr"/>
@@ -829,7 +829,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-A11', 'Hhx heat exchanger [USD]')</t>
+          <t>('Hydronic heat exchanger-A11', 'Hydronic heat exchanger hhx heat exchanger [USD]')</t>
         </is>
       </c>
       <c r="C24" t="inlineStr"/>
@@ -845,7 +845,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-A11', 'Hhx values [USD]')</t>
+          <t>('Hydronic heat exchanger-A11', 'Hydronic heat exchanger hhx values [USD]')</t>
         </is>
       </c>
       <c r="C25" t="inlineStr"/>
@@ -861,7 +861,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-A11', 'Hhx thermal well [USD]')</t>
+          <t>('Hydronic heat exchanger-A11', 'Hydronic heat exchanger hhx thermal well [USD]')</t>
         </is>
       </c>
       <c r="C26" t="inlineStr"/>
@@ -877,7 +877,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-A11', 'Hhx hot water tank [USD]')</t>
+          <t>('Hydronic heat exchanger-A11', 'Hydronic heat exchanger hhx hot water tank [USD]')</t>
         </is>
       </c>
       <c r="C27" t="inlineStr"/>
@@ -893,7 +893,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-A11', 'Hhx overflow tank [USD]')</t>
+          <t>('Hydronic heat exchanger-A11', 'Hydronic heat exchanger hhx overflow tank [USD]')</t>
         </is>
       </c>
       <c r="C28" t="inlineStr"/>
@@ -909,7 +909,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-A11', 'Steel cost [USD/kg]')</t>
+          <t>('Hydronic heat exchanger-A11', 'Hydronic heat exchanger steel cost [USD/kg]')</t>
         </is>
       </c>
       <c r="C29" t="inlineStr"/>
@@ -925,7 +925,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-A11', 'Stainless steel cost [USD/kg]')</t>
+          <t>('Hydronic heat exchanger-A11', 'Hydronic heat exchanger stainless steel cost [USD/kg]')</t>
         </is>
       </c>
       <c r="C30" t="inlineStr"/>
@@ -941,7 +941,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-A11', 'Frequency corrective maintenance [y / occurance]')</t>
+          <t>('Hydronic heat exchanger-A11', 'Hydronic heat exchanger frequency corrective maintenance [y / occurance]')</t>
         </is>
       </c>
       <c r="C31" t="inlineStr"/>
@@ -957,7 +957,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-A11', 'Service team adjustdoor hhx [min / month]')</t>
+          <t>('Hydronic heat exchanger-A11', 'Hydronic heat exchanger service team adjustdoor hhx [min / month]')</t>
         </is>
       </c>
       <c r="C32" t="inlineStr"/>
@@ -973,7 +973,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-A11', 'Service team replacewaterpump hhx [min / corrective maintenance]')</t>
+          <t>('Hydronic heat exchanger-A11', 'Hydronic heat exchanger service team replacewaterpump hhx [min / corrective maintenance]')</t>
         </is>
       </c>
       <c r="C33" t="inlineStr"/>
@@ -989,7 +989,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-A11', 'Service team purgewaterloop hhx [min / corrective maintenance]')</t>
+          <t>('Hydronic heat exchanger-A11', 'Hydronic heat exchanger service team purgewaterloop hhx [min / corrective maintenance]')</t>
         </is>
       </c>
       <c r="C34" t="inlineStr"/>
@@ -1005,7 +1005,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-A11', 'Hhx temp [C]')</t>
+          <t>('Hydronic heat exchanger-A11', 'Hydronic heat exchanger hhx temp [C]')</t>
         </is>
       </c>
       <c r="C35" t="inlineStr"/>
@@ -1021,7 +1021,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-A11', 'Water flowrate [L/min]')</t>
+          <t>('Hydronic heat exchanger-A11', 'Hydronic heat exchanger water flowrate [L/min]')</t>
         </is>
       </c>
       <c r="C36" t="inlineStr"/>
@@ -1037,7 +1037,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-A11', 'Water out temp [C]')</t>
+          <t>('Hydronic heat exchanger-A11', 'Hydronic heat exchanger water out temp [C]')</t>
         </is>
       </c>
       <c r="C37" t="inlineStr"/>
@@ -1053,7 +1053,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-A11', 'Water in temp [C]')</t>
+          <t>('Hydronic heat exchanger-A11', 'Hydronic heat exchanger water in temp [C]')</t>
         </is>
       </c>
       <c r="C38" t="inlineStr"/>
@@ -1069,7 +1069,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-A11', 'Ambient temp [C]')</t>
+          <t>('Hydronic heat exchanger-A11', 'Hydronic heat exchanger ambient temp [C]')</t>
         </is>
       </c>
       <c r="C39" t="inlineStr"/>
@@ -1085,7 +1085,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>('HHXdryer-A12', 'Drying energy demand [kW]')</t>
+          <t>('HHXdryer-A12', 'HHXdryer drying energy demand [kW]')</t>
         </is>
       </c>
       <c r="C40" t="inlineStr"/>
@@ -1101,7 +1101,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>('HHXdryer-A12', 'Drying co2 emissions [% of total C]')</t>
+          <t>('HHXdryer-A12', 'HHXdryer drying co2 emissions [% of total C]')</t>
         </is>
       </c>
       <c r="C41" t="inlineStr"/>
@@ -1117,7 +1117,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>('HHXdryer-A12', 'Drying ch4 emissions [% of total C]')</t>
+          <t>('HHXdryer-A12', 'HHXdryer drying ch4 emissions [% of total C]')</t>
         </is>
       </c>
       <c r="C42" t="inlineStr"/>
@@ -1133,7 +1133,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>('HHXdryer-A12', 'Drying nh3 emissions [% of total N]')</t>
+          <t>('HHXdryer-A12', 'HHXdryer drying nh3 emissions [% of total N]')</t>
         </is>
       </c>
       <c r="C43" t="inlineStr"/>
@@ -1149,7 +1149,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>('HHXdryer-A12', 'NH3 to n2o [% of NH3]')</t>
+          <t>('HHXdryer-A12', 'HHXdryer nh3 to n2o [% of NH3]')</t>
         </is>
       </c>
       <c r="C44" t="inlineStr"/>
@@ -1165,7 +1165,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>('HHXdryer-A12', 'Energy required to dry sludge [MJ/kg water]')</t>
+          <t>('HHXdryer-A12', 'HHXdryer energy required to dry sludge [MJ/kg water]')</t>
         </is>
       </c>
       <c r="C45" t="inlineStr"/>
@@ -1181,7 +1181,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>('HHXdryer-A12', 'Ambient temp [C]')</t>
+          <t>('HHXdryer-A12', 'HHXdryer ambient temp [C]')</t>
         </is>
       </c>
       <c r="C46" t="inlineStr"/>
@@ -1197,7 +1197,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>('HHXdryer-A12', 'Dryer heat transfer coeff [MJ / (h m2 K)]')</t>
+          <t>('HHXdryer-A12', 'HHXdryer dryer heat transfer coeff [MJ / (h m2 K)]')</t>
         </is>
       </c>
       <c r="C47" t="inlineStr"/>
@@ -1213,7 +1213,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>('HHXdryer-A12', 'Water out temp [C]')</t>
+          <t>('HHXdryer-A12', 'HHXdryer water out temp [C]')</t>
         </is>
       </c>
       <c r="C48" t="inlineStr"/>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>('HHXdryer-A12', 'Carbon COD ratio [g C*g COD-1]')</t>
+          <t>('HHXdryer-A12', 'HHXdryer carbon COD ratio [g C*g COD-1]')</t>
         </is>
       </c>
       <c r="C49" t="inlineStr"/>
@@ -1245,7 +1245,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'N prot [fraction]')</t>
+          <t>('Excretion-A1', 'Excretion N prot [fraction]')</t>
         </is>
       </c>
       <c r="C50" t="inlineStr"/>
@@ -1261,7 +1261,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'P prot v [fraction]')</t>
+          <t>('Excretion-A1', 'Excretion P prot v [fraction]')</t>
         </is>
       </c>
       <c r="C51" t="inlineStr"/>
@@ -1277,7 +1277,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'P prot a [fraction]')</t>
+          <t>('Excretion-A1', 'Excretion P prot a [fraction]')</t>
         </is>
       </c>
       <c r="C52" t="inlineStr"/>
@@ -1293,7 +1293,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'K cal [g K/1000 kcal]')</t>
+          <t>('Excretion-A1', 'Excretion K cal [g K/1000 kcal]')</t>
         </is>
       </c>
       <c r="C53" t="inlineStr"/>
@@ -1309,7 +1309,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'N exc [fraction of intake]')</t>
+          <t>('Excretion-A1', 'Excretion N exc [fraction of intake]')</t>
         </is>
       </c>
       <c r="C54" t="inlineStr"/>
@@ -1325,7 +1325,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'P exc [fraction of intake]')</t>
+          <t>('Excretion-A1', 'Excretion P exc [fraction of intake]')</t>
         </is>
       </c>
       <c r="C55" t="inlineStr"/>
@@ -1341,7 +1341,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'K exc [fraction of intake]')</t>
+          <t>('Excretion-A1', 'Excretion K exc [fraction of intake]')</t>
         </is>
       </c>
       <c r="C56" t="inlineStr"/>
@@ -1357,7 +1357,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'E exc [fraction of intake]')</t>
+          <t>('Excretion-A1', 'Excretion e exc [fraction of intake]')</t>
         </is>
       </c>
       <c r="C57" t="inlineStr"/>
@@ -1373,7 +1373,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'N ur [fraction of total]')</t>
+          <t>('Excretion-A1', 'Excretion N ur [fraction of total]')</t>
         </is>
       </c>
       <c r="C58" t="inlineStr"/>
@@ -1389,7 +1389,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'P ur [fraction of total]')</t>
+          <t>('Excretion-A1', 'Excretion P ur [fraction of total]')</t>
         </is>
       </c>
       <c r="C59" t="inlineStr"/>
@@ -1405,7 +1405,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'K ur [fraction of total]')</t>
+          <t>('Excretion-A1', 'Excretion K ur [fraction of total]')</t>
         </is>
       </c>
       <c r="C60" t="inlineStr"/>
@@ -1421,7 +1421,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'E fec [fraction of total]')</t>
+          <t>('Excretion-A1', 'Excretion e fec [fraction of total]')</t>
         </is>
       </c>
       <c r="C61" t="inlineStr"/>
@@ -1437,7 +1437,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'N ur NH3 [fraction of total N in urine]')</t>
+          <t>('Excretion-A1', 'Excretion N ur NH3 [fraction of total N in urine]')</t>
         </is>
       </c>
       <c r="C62" t="inlineStr"/>
@@ -1453,7 +1453,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'N fec NH3 [fraction of total N in feces]')</t>
+          <t>('Excretion-A1', 'Excretion N fec NH3 [fraction of total N in feces]')</t>
         </is>
       </c>
       <c r="C63" t="inlineStr"/>
@@ -1469,7 +1469,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'Ur exc [g/cap/d]')</t>
+          <t>('Excretion-A1', 'Excretion ur exc [g/cap/d]')</t>
         </is>
       </c>
       <c r="C64" t="inlineStr"/>
@@ -1485,7 +1485,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'Fec exc [g/cap/d]')</t>
+          <t>('Excretion-A1', 'Excretion fec exc [g/cap/d]')</t>
         </is>
       </c>
       <c r="C65" t="inlineStr"/>
@@ -1501,7 +1501,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'Ur moi [fraction]')</t>
+          <t>('Excretion-A1', 'Excretion ur moi [fraction]')</t>
         </is>
       </c>
       <c r="C66" t="inlineStr"/>
@@ -1517,7 +1517,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'Fec moi [fraction]')</t>
+          <t>('Excretion-A1', 'Excretion fec moi [fraction]')</t>
         </is>
       </c>
       <c r="C67" t="inlineStr"/>
@@ -1533,7 +1533,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'Mg ur [g Mg/cap/d]')</t>
+          <t>('Excretion-A1', 'Excretion mg ur [g Mg/cap/d]')</t>
         </is>
       </c>
       <c r="C68" t="inlineStr"/>
@@ -1549,7 +1549,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'Mg fec [g Mg/cap/d]')</t>
+          <t>('Excretion-A1', 'Excretion mg fec [g Mg/cap/d]')</t>
         </is>
       </c>
       <c r="C69" t="inlineStr"/>
@@ -1565,7 +1565,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'Ca ur [g Ca/cap/d]')</t>
+          <t>('Excretion-A1', 'Excretion ca ur [g Ca/cap/d]')</t>
         </is>
       </c>
       <c r="C70" t="inlineStr"/>
@@ -1581,7 +1581,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>('Excretion-A1', 'Ca fec [g Ca/cap/d]')</t>
+          <t>('Excretion-A1', 'Excretion ca fec [g Ca/cap/d]')</t>
         </is>
       </c>
       <c r="C71" t="inlineStr"/>
@@ -1741,7 +1741,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>('Pit latrine-A2', 'Toilet paper [kg/cap/hr]')</t>
+          <t>('Pit latrine-A2', 'Pit latrine toilet paper [kg/cap/hr]')</t>
         </is>
       </c>
       <c r="C81" t="inlineStr"/>
@@ -1757,7 +1757,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>('Pit latrine-A2', 'Flushing water [kg/cap/hr]')</t>
+          <t>('Pit latrine-A2', 'Pit latrine flushing water [kg/cap/hr]')</t>
         </is>
       </c>
       <c r="C82" t="inlineStr"/>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>('Pit latrine-A2', 'Cleansing water [kg/cap/hr]')</t>
+          <t>('Pit latrine-A2', 'Pit latrine cleansing water [kg/cap/hr]')</t>
         </is>
       </c>
       <c r="C83" t="inlineStr"/>
@@ -1789,7 +1789,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>('Pit latrine-A2', 'Desiccant V [m3/cap/hr]')</t>
+          <t>('Pit latrine-A2', 'Pit latrine desiccant V [m3/cap/hr]')</t>
         </is>
       </c>
       <c r="C84" t="inlineStr"/>
@@ -1805,7 +1805,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>('Pit latrine-A2', 'Desiccant rho [kg/m3]')</t>
+          <t>('Pit latrine-A2', 'Pit latrine desiccant rho [kg/m3]')</t>
         </is>
       </c>
       <c r="C85" t="inlineStr"/>
@@ -1821,7 +1821,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>('Pit latrine-A2', 'COD max decay [fraction of oxygen demand removal]')</t>
+          <t>('Pit latrine-A2', 'Pit latrine COD max decay [fraction of oxygen demand removal]')</t>
         </is>
       </c>
       <c r="C86" t="inlineStr"/>
@@ -1837,7 +1837,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>('Pit latrine-A2', 'N max decay [fraction of N removal after N leaching]')</t>
+          <t>('Pit latrine-A2', 'Pit latrine N max decay [fraction of N removal after N leaching]')</t>
         </is>
       </c>
       <c r="C87" t="inlineStr"/>
@@ -1853,7 +1853,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>('Pit latrine-A2', 'MCF aq [fraction of anaerobic conversion of degraded COD]')</t>
+          <t>('Pit latrine-A2', 'Pit latrine MCF aq [fraction of anaerobic conversion of degraded COD]')</t>
         </is>
       </c>
       <c r="C88" t="inlineStr"/>
@@ -1869,7 +1869,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>('Pit latrine-A2', 'N2O EF aq [fraction of N emitted as N2O]')</t>
+          <t>('Pit latrine-A2', 'Pit latrine n2o EF aq [fraction of N emitted as N2O]')</t>
         </is>
       </c>
       <c r="C89" t="inlineStr"/>
@@ -1885,7 +1885,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>('Pit latrine-A2', 'Emptying period [yr]')</t>
+          <t>('Pit latrine-A2', 'Pit latrine emptying period [yr]')</t>
         </is>
       </c>
       <c r="C90" t="inlineStr"/>
@@ -1901,7 +1901,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>('Pit latrine-A2', 'Sludge accum rate [L/cap/yr]')</t>
+          <t>('Pit latrine-A2', 'Pit latrine sludge accum rate [L/cap/yr]')</t>
         </is>
       </c>
       <c r="C91" t="inlineStr"/>
@@ -1917,7 +1917,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>('Pit latrine-A2', 'N leaching [fraction of N input]')</t>
+          <t>('Pit latrine-A2', 'Pit latrine N leaching [fraction of N input]')</t>
         </is>
       </c>
       <c r="C92" t="inlineStr"/>
@@ -1933,7 +1933,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>('Pit latrine-A2', 'P leaching [fraction of P input]')</t>
+          <t>('Pit latrine-A2', 'Pit latrine P leaching [fraction of P input]')</t>
         </is>
       </c>
       <c r="C93" t="inlineStr"/>
@@ -1949,7 +1949,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>('Pit latrine-A2', 'K leaching [fraction of K input]')</t>
+          <t>('Pit latrine-A2', 'Pit latrine K leaching [fraction of K input]')</t>
         </is>
       </c>
       <c r="C94" t="inlineStr"/>
@@ -1965,7 +1965,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>('Pit latrine-A2', 'N volatilization [fraction of N input]')</t>
+          <t>('Pit latrine-A2', 'Pit latrine N volatilization [fraction of N input]')</t>
         </is>
       </c>
       <c r="C95" t="inlineStr"/>
@@ -2189,7 +2189,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>('Control box OP-A4', 'Icp controller board [USD]')</t>
+          <t>('Control box OP-A4', 'Control box OP icp controller board [USD]')</t>
         </is>
       </c>
       <c r="C109" t="inlineStr"/>
@@ -2205,7 +2205,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>('Control box OP-A4', 'Icp variable frequence drives [USD]')</t>
+          <t>('Control box OP-A4', 'Control box OP icp variable frequence drives [USD]')</t>
         </is>
       </c>
       <c r="C110" t="inlineStr"/>
@@ -2221,7 +2221,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>('Control box OP-A4', 'Icp power meter [USD]')</t>
+          <t>('Control box OP-A4', 'Control box OP icp power meter [USD]')</t>
         </is>
       </c>
       <c r="C111" t="inlineStr"/>
@@ -2237,7 +2237,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>('Control box OP-A4', 'Icp line filter [USD]')</t>
+          <t>('Control box OP-A4', 'Control box OP icp line filter [USD]')</t>
         </is>
       </c>
       <c r="C112" t="inlineStr"/>
@@ -2253,7 +2253,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>('Control box OP-A4', 'Icp power meter transformer [USD]')</t>
+          <t>('Control box OP-A4', 'Control box OP icp power meter transformer [USD]')</t>
         </is>
       </c>
       <c r="C113" t="inlineStr"/>
@@ -2269,7 +2269,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>('Control box OP-A4', 'Icp touch screen [USD]')</t>
+          <t>('Control box OP-A4', 'Control box OP icp touch screen [USD]')</t>
         </is>
       </c>
       <c r="C114" t="inlineStr"/>
@@ -2285,7 +2285,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>('Control box OP-A4', 'Electrician replacecables icp [nan]')</t>
+          <t>('Control box OP-A4', 'Control box OP electrician replacecables icp [nan]')</t>
         </is>
       </c>
       <c r="C115" t="inlineStr"/>
@@ -2301,7 +2301,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>('Control box OP-A4', 'Electrician replacewires icp [nan]')</t>
+          <t>('Control box OP-A4', 'Control box OP electrician replacewires icp [nan]')</t>
         </is>
       </c>
       <c r="C116" t="inlineStr"/>
@@ -2317,7 +2317,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>('Control box OP-A4', 'Service team replacetouchscreen icp [nan]')</t>
+          <t>('Control box OP-A4', 'Control box OP service team replacetouchscreen icp [nan]')</t>
         </is>
       </c>
       <c r="C117" t="inlineStr"/>
@@ -2333,7 +2333,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>('Control box OP-A4', 'Facility manager configurevariable icp [nan]')</t>
+          <t>('Control box OP-A4', 'Control box OP facility manager configurevariable icp [nan]')</t>
         </is>
       </c>
       <c r="C118" t="inlineStr"/>
@@ -2349,7 +2349,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>('Control box OP-A4', 'Biomass controls replaceboard icp [nan]')</t>
+          <t>('Control box OP-A4', 'Control box OP biomass controls replaceboard icp [nan]')</t>
         </is>
       </c>
       <c r="C119" t="inlineStr"/>
@@ -2365,7 +2365,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>('Control box OP-A4', 'Biomass controls codemalfunctioning icp [nan]')</t>
+          <t>('Control box OP-A4', 'Control box OP biomass controls codemalfunctioning icp [nan]')</t>
         </is>
       </c>
       <c r="C120" t="inlineStr"/>
@@ -2381,7 +2381,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>('Control box OP-A4', 'Frequency corrective maintenance [y / occurance]')</t>
+          <t>('Control box OP-A4', 'Control box OP frequency corrective maintenance [y / occurance]')</t>
         </is>
       </c>
       <c r="C121" t="inlineStr"/>
@@ -2397,7 +2397,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>('Housing biogenic refinery-A5', 'Container20ft cost [USD]')</t>
+          <t>('Housing biogenic refinery-A5', 'Housing biogenic refinery container20ft cost [USD]')</t>
         </is>
       </c>
       <c r="C122" t="inlineStr"/>
@@ -2413,7 +2413,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>('Housing biogenic refinery-A5', 'Container40ft cost [USD]')</t>
+          <t>('Housing biogenic refinery-A5', 'Housing biogenic refinery container40ft cost [USD]')</t>
         </is>
       </c>
       <c r="C123" t="inlineStr"/>
@@ -2429,7 +2429,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>('Housing biogenic refinery-A5', 'Stainless steel housing [USD per m2]')</t>
+          <t>('Housing biogenic refinery-A5', 'Housing biogenic refinery stainless steel housing [USD per m2]')</t>
         </is>
       </c>
       <c r="C124" t="inlineStr"/>
@@ -2445,7 +2445,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>('Housing biogenic refinery-A5', 'Concrete cost [USD per m3]')</t>
+          <t>('Housing biogenic refinery-A5', 'Housing biogenic refinery concrete cost [USD per m3]')</t>
         </is>
       </c>
       <c r="C125" t="inlineStr"/>
@@ -2461,7 +2461,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>('Housing biogenic refinery-A5', 'Concrete thickness [m]')</t>
+          <t>('Housing biogenic refinery-A5', 'Housing biogenic refinery concrete thickness [m]')</t>
         </is>
       </c>
       <c r="C126" t="inlineStr"/>
@@ -2477,7 +2477,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>('Housing biogenic refinery-A5', 'Footprint [m2]')</t>
+          <t>('Housing biogenic refinery-A5', 'Housing biogenic refinery footprint [m2]')</t>
         </is>
       </c>
       <c r="C127" t="inlineStr"/>
@@ -2493,7 +2493,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>('Screw press-A6', 'Dewatering screw press cost [usd]')</t>
+          <t>('Screw press-A6', 'Screw press dewatering screw press cost [usd]')</t>
         </is>
       </c>
       <c r="C128" t="inlineStr"/>
@@ -2509,7 +2509,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>('Screw press-A6', 'Dewatering screw press steel [kg]')</t>
+          <t>('Screw press-A6', 'Screw press dewatering screw press steel [kg]')</t>
         </is>
       </c>
       <c r="C129" t="inlineStr"/>
@@ -2525,7 +2525,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>('Screw press-A6', 'Dewatering energy demand [kwh/kg solids]')</t>
+          <t>('Screw press-A6', 'Screw press dewatering energy demand [kwh/kg solids]')</t>
         </is>
       </c>
       <c r="C130" t="inlineStr"/>
@@ -2541,7 +2541,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>('Screw press-A6', 'Dewatering polymer dose [g/kg dry TS]')</t>
+          <t>('Screw press-A6', 'Screw press dewatering polymer dose [g/kg dry TS]')</t>
         </is>
       </c>
       <c r="C131" t="inlineStr"/>
@@ -2557,7 +2557,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>('Screw press-A6', 'Cake solids TS [fraction]')</t>
+          <t>('Screw press-A6', 'Screw press cake solids TS [fraction]')</t>
         </is>
       </c>
       <c r="C132" t="inlineStr"/>
@@ -2573,7 +2573,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>('Screw press-A6', 'Settled frac [fraction]')</t>
+          <t>('Screw press-A6', 'Screw press  settled frac [fraction]')</t>
         </is>
       </c>
       <c r="C133" t="inlineStr"/>
@@ -2589,7 +2589,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>('Screw press-A6', 'Wwt cost [usd per m3]')</t>
+          <t>('Screw press-A6', 'Screw press wwt cost [usd per m3]')</t>
         </is>
       </c>
       <c r="C134" t="inlineStr"/>
@@ -2605,7 +2605,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>('Screw press-A6', 'Polymer cost [usd per kg]')</t>
+          <t>('Screw press-A6', 'Screw press polymer cost [usd per kg]')</t>
         </is>
       </c>
       <c r="C135" t="inlineStr"/>
@@ -2621,7 +2621,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>('Liquid treatment bed-A7', 'Tau [d]')</t>
+          <t>('Liquid treatment bed-A7', 'Liquid treatment bed tau [d]')</t>
         </is>
       </c>
       <c r="C136" t="inlineStr"/>
@@ -2637,7 +2637,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>('Liquid treatment bed-A7', 'COD max decay [% of total COD]')</t>
+          <t>('Liquid treatment bed-A7', 'Liquid treatment bed COD max decay [% of total COD]')</t>
         </is>
       </c>
       <c r="C137" t="inlineStr"/>
@@ -2653,7 +2653,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>('Liquid treatment bed-A7', 'MCF decay [% anaerobic conversion of degraded COD]')</t>
+          <t>('Liquid treatment bed-A7', 'Liquid treatment bed MCF decay [% anaerobic conversion of degraded COD]')</t>
         </is>
       </c>
       <c r="C138" t="inlineStr"/>
@@ -2669,7 +2669,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>('Liquid treatment bed-A7', 'N max decay [% N removal]')</t>
+          <t>('Liquid treatment bed-A7', 'Liquid treatment bed N max decay [% N removal]')</t>
         </is>
       </c>
       <c r="C139" t="inlineStr"/>
@@ -2685,7 +2685,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>('Liquid treatment bed-A7', 'N2O EF decay [% of degraded N emitted as N2O]')</t>
+          <t>('Liquid treatment bed-A7', 'Liquid treatment bed n2o EF decay [% of degraded N emitted as N2O]')</t>
         </is>
       </c>
       <c r="C140" t="inlineStr"/>
@@ -2701,7 +2701,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>('Liquid treatment bed-A7', 'Bed H [m]')</t>
+          <t>('Liquid treatment bed-A7', 'Liquid treatment bed bed H [m]')</t>
         </is>
       </c>
       <c r="C141" t="inlineStr"/>
@@ -2717,7 +2717,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>('Liquid treatment bed-A7', 'Concrete thickness [m]')</t>
+          <t>('Liquid treatment bed-A7', 'Liquid treatment bed concrete thickness [m]')</t>
         </is>
       </c>
       <c r="C142" t="inlineStr"/>
@@ -2733,7 +2733,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Energy required to dry sludge [MJ/kg water]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base energy required to dry sludge [MJ/kg water]')</t>
         </is>
       </c>
       <c r="C143" t="inlineStr"/>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Dry feces heat of combustion [MJ/kg dry]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base dry feces heat of combustion [MJ/kg dry]')</t>
         </is>
       </c>
       <c r="C144" t="inlineStr"/>
@@ -2765,7 +2765,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Pyrolysis pot cost cb [USD]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base pyrolysis pot cost cb [USD]')</t>
         </is>
       </c>
       <c r="C145" t="inlineStr"/>
@@ -2781,7 +2781,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Char auger motor cost cb [USD]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base char auger motor cost cb [USD]')</t>
         </is>
       </c>
       <c r="C146" t="inlineStr"/>
@@ -2797,7 +2797,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Fuel auger motor cost cb [USD]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base fuel auger motor cost cb [USD]')</t>
         </is>
       </c>
       <c r="C147" t="inlineStr"/>
@@ -2813,7 +2813,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Primary air blower cost cb [USD]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base primary air blower cost cb [USD]')</t>
         </is>
       </c>
       <c r="C148" t="inlineStr"/>
@@ -2829,7 +2829,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Thermocouple cost cb pcd [USD]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base thermocouple cost cb pcd [USD]')</t>
         </is>
       </c>
       <c r="C149" t="inlineStr"/>
@@ -2845,7 +2845,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Thermistor cost cb pcd [USD]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base thermistor cost cb pcd [USD]')</t>
         </is>
       </c>
       <c r="C150" t="inlineStr"/>
@@ -2861,7 +2861,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Forced air fan cost cb [USD]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base forced air fan cost cb [USD]')</t>
         </is>
       </c>
       <c r="C151" t="inlineStr"/>
@@ -2877,7 +2877,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Airlock motor cost cb [USD]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base airlock motor cost cb [USD]')</t>
         </is>
       </c>
       <c r="C152" t="inlineStr"/>
@@ -2893,7 +2893,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Inducer fan cost cb [USD]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base inducer fan cost cb [USD]')</t>
         </is>
       </c>
       <c r="C153" t="inlineStr"/>
@@ -2909,7 +2909,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Biochar collection box cost cb [USD]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base biochar collection box cost cb [USD]')</t>
         </is>
       </c>
       <c r="C154" t="inlineStr"/>
@@ -2925,7 +2925,7 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Chain guards cost cb [USD]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base chain guards cost cb [USD]')</t>
         </is>
       </c>
       <c r="C155" t="inlineStr"/>
@@ -2941,7 +2941,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Door cost cb [USD]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base door cost cb [USD]')</t>
         </is>
       </c>
       <c r="C156" t="inlineStr"/>
@@ -2957,7 +2957,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Agitator cost cb [USD]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base agitator cost cb [USD]')</t>
         </is>
       </c>
       <c r="C157" t="inlineStr"/>
@@ -2973,7 +2973,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Combusion chamber cost cb [USD]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base combusion chamber cost cb [USD]')</t>
         </is>
       </c>
       <c r="C158" t="inlineStr"/>
@@ -2989,7 +2989,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Sprayer cost cb [USD]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base sprayer cost cb [USD]')</t>
         </is>
       </c>
       <c r="C159" t="inlineStr"/>
@@ -3005,7 +3005,7 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Vent cost cb [USD]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base vent cost cb [USD]')</t>
         </is>
       </c>
       <c r="C160" t="inlineStr"/>
@@ -3021,7 +3021,7 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'SO2 emissions [mg/Nm3]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base so2 emissions [mg/Nm3]')</t>
         </is>
       </c>
       <c r="C161" t="inlineStr"/>
@@ -3037,7 +3037,7 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'CO emissions [mg/Nm3]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base CO emissions [mg/Nm3]')</t>
         </is>
       </c>
       <c r="C162" t="inlineStr"/>
@@ -3053,7 +3053,7 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Hg emissions [mg/Nm3]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base hg emissions [mg/Nm3]')</t>
         </is>
       </c>
       <c r="C163" t="inlineStr"/>
@@ -3069,7 +3069,7 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Cd emissions [mg/Nm3]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base cd emissions [mg/Nm3]')</t>
         </is>
       </c>
       <c r="C164" t="inlineStr"/>
@@ -3085,7 +3085,7 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'As emissions [mg/Nm3]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base as emissions [mg/Nm3]')</t>
         </is>
       </c>
       <c r="C165" t="inlineStr"/>
@@ -3101,7 +3101,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Dioxin furans emissions [ng/Nm3]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base dioxin furans emissions [ng/Nm3]')</t>
         </is>
       </c>
       <c r="C166" t="inlineStr"/>
@@ -3117,7 +3117,7 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Cb n2o emissions [% of total N]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base cb n2o emissions [% of total N]')</t>
         </is>
       </c>
       <c r="C167" t="inlineStr"/>
@@ -3133,7 +3133,7 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Steel cost [USD/kg]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base steel cost [USD/kg]')</t>
         </is>
       </c>
       <c r="C168" t="inlineStr"/>
@@ -3149,7 +3149,7 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Stainless steel cost [USD/kg]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base stainless steel cost [USD/kg]')</t>
         </is>
       </c>
       <c r="C169" t="inlineStr"/>
@@ -3165,7 +3165,7 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Primary air blower lifetime cb [y]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base primary air blower lifetime cb [y]')</t>
         </is>
       </c>
       <c r="C170" t="inlineStr"/>
@@ -3181,7 +3181,7 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Thermocouple lifetime cb 2pcd [y]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base thermocouple lifetime cb 2pcd [y]')</t>
         </is>
       </c>
       <c r="C171" t="inlineStr"/>
@@ -3197,7 +3197,7 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Forced air fan lifetime cb [y]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base forced air fan lifetime cb [y]')</t>
         </is>
       </c>
       <c r="C172" t="inlineStr"/>
@@ -3213,7 +3213,7 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Airlock motor lifetime cb [y]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base airlock motor lifetime cb [y]')</t>
         </is>
       </c>
       <c r="C173" t="inlineStr"/>
@@ -3229,7 +3229,7 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Inducer fan lifetime cb [y]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base inducer fan lifetime cb [y]')</t>
         </is>
       </c>
       <c r="C174" t="inlineStr"/>
@@ -3245,7 +3245,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Service team replacegasket cb [min / corrective maintenance]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base service team replacegasket cb [min / corrective maintenance]')</t>
         </is>
       </c>
       <c r="C175" t="inlineStr"/>
@@ -3261,7 +3261,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Service team replacedoor cb [min / corrective maintenance]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base service team replacedoor cb [min / corrective maintenance]')</t>
         </is>
       </c>
       <c r="C176" t="inlineStr"/>
@@ -3277,7 +3277,7 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Service team replacechain cb [min / corrective maintenance]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base service team replacechain cb [min / corrective maintenance]')</t>
         </is>
       </c>
       <c r="C177" t="inlineStr"/>
@@ -3293,7 +3293,7 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Service team changefirepot cb [min / corrective maintenance]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base service team changefirepot cb [min / corrective maintenance]')</t>
         </is>
       </c>
       <c r="C178" t="inlineStr"/>
@@ -3309,7 +3309,7 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Service team replacecharaugers cb [min / corrective maintenance]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base service team replacecharaugers cb [min / corrective maintenance]')</t>
         </is>
       </c>
       <c r="C179" t="inlineStr"/>
@@ -3325,7 +3325,7 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Service team replacecatalyst pcd [min / corrective maintenance]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base service team replacecatalyst pcd [min / corrective maintenance]')</t>
         </is>
       </c>
       <c r="C180" t="inlineStr"/>
@@ -3341,7 +3341,7 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Service team replacebrick pcd [min / corrective maintenance]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base service team replacebrick pcd [min / corrective maintenance]')</t>
         </is>
       </c>
       <c r="C181" t="inlineStr"/>
@@ -3357,7 +3357,7 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Service team replacefuelauger pcd [min / corrective maintenance]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base service team replacefuelauger pcd [min / corrective maintenance]')</t>
         </is>
       </c>
       <c r="C182" t="inlineStr"/>
@@ -3373,7 +3373,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Service team replacewaterpump hhx [min / corrective maintenance]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base service team replacewaterpump hhx [min / corrective maintenance]')</t>
         </is>
       </c>
       <c r="C183" t="inlineStr"/>
@@ -3389,7 +3389,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Service team purgewaterloop hhx [min / corrective maintenance]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base service team purgewaterloop hhx [min / corrective maintenance]')</t>
         </is>
       </c>
       <c r="C184" t="inlineStr"/>
@@ -3405,7 +3405,7 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Service team replacecharmotor cb [min / corrective maintenance]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base service team replacecharmotor cb [min / corrective maintenance]')</t>
         </is>
       </c>
       <c r="C185" t="inlineStr"/>
@@ -3421,7 +3421,7 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Service team replacefuelmotor cb [min / corrective maintenance]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base service team replacefuelmotor cb [min / corrective maintenance]')</t>
         </is>
       </c>
       <c r="C186" t="inlineStr"/>
@@ -3437,7 +3437,7 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Service team replaceblower cb [min / corrective maintenance]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base service team replaceblower cb [min / corrective maintenance]')</t>
         </is>
       </c>
       <c r="C187" t="inlineStr"/>
@@ -3453,7 +3453,7 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Service team replacefan cb [min / corrective maintenance]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base service team replacefan cb [min / corrective maintenance]')</t>
         </is>
       </c>
       <c r="C188" t="inlineStr"/>
@@ -3469,7 +3469,7 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Service team replaceo2sensor pcd [min / corrective maintenance]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base service team replaceo2sensor pcd [min / corrective maintenance]')</t>
         </is>
       </c>
       <c r="C189" t="inlineStr"/>
@@ -3485,7 +3485,7 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Service team replacepaddleswitch cb [min / corrective maintenance]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base service team replacepaddleswitch cb [min / corrective maintenance]')</t>
         </is>
       </c>
       <c r="C190" t="inlineStr"/>
@@ -3501,7 +3501,7 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Service team replaceairlock cb [min / corrective maintenance]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base service team replaceairlock cb [min / corrective maintenance]')</t>
         </is>
       </c>
       <c r="C191" t="inlineStr"/>
@@ -3517,7 +3517,7 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Service team greasebearing cb [min / month]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base service team greasebearing cb [min / month]')</t>
         </is>
       </c>
       <c r="C192" t="inlineStr"/>
@@ -3533,7 +3533,7 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Service team tighten cb [min / month]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base service team tighten cb [min / month]')</t>
         </is>
       </c>
       <c r="C193" t="inlineStr"/>
@@ -3549,7 +3549,7 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Service team adjustdoor cb [min / month]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base service team adjustdoor cb [min / month]')</t>
         </is>
       </c>
       <c r="C194" t="inlineStr"/>
@@ -3565,7 +3565,7 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Service team adjustdoor pcd [min / month]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base service team adjustdoor pcd [min / month]')</t>
         </is>
       </c>
       <c r="C195" t="inlineStr"/>
@@ -3581,7 +3581,7 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Service team adjustdoor hhx [min / month]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base service team adjustdoor hhx [min / month]')</t>
         </is>
       </c>
       <c r="C196" t="inlineStr"/>
@@ -3597,7 +3597,7 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Frequency corrective maintenance [y / occurance]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base frequency corrective maintenance [y / occurance]')</t>
         </is>
       </c>
       <c r="C197" t="inlineStr"/>
@@ -3613,7 +3613,7 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Biochar calorific value [MJ/kg dry]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base biochar calorific value [MJ/kg dry]')</t>
         </is>
       </c>
       <c r="C198" t="inlineStr"/>
@@ -3629,7 +3629,7 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Pyrolysis temp [C]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base pyrolysis temp [C]')</t>
         </is>
       </c>
       <c r="C199" t="inlineStr"/>
@@ -3645,7 +3645,7 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Pyrolysis C loss [fraction of total C]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base pyrolysis C loss [fraction of total C]')</t>
         </is>
       </c>
       <c r="C200" t="inlineStr"/>
@@ -3661,7 +3661,7 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Pyrolysis N loss [fraction of total N]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base pyrolysis N loss [fraction of total N]')</t>
         </is>
       </c>
       <c r="C201" t="inlineStr"/>
@@ -3677,7 +3677,7 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Pyrolysis K loss [fraction of total K]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base pyrolysis K loss [fraction of total K]')</t>
         </is>
       </c>
       <c r="C202" t="inlineStr"/>
@@ -3693,7 +3693,7 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Pyrolysis P loss [fraction of total P]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base pyrolysis P loss [fraction of total P]')</t>
         </is>
       </c>
       <c r="C203" t="inlineStr"/>
@@ -3709,7 +3709,7 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'N to NH3 [fraction of N]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer Base N to NH3 [fraction of N]')</t>
         </is>
       </c>
       <c r="C204" t="inlineStr"/>
@@ -3725,7 +3725,7 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'N to HCNO [fraction of N]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base N to HCNO [fraction of N]')</t>
         </is>
       </c>
       <c r="C205" t="inlineStr"/>
@@ -3741,7 +3741,7 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'HCNO to NH3 [fraction of HCNO]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer Base HCNO to NH3 [fraction of HCNO]')</t>
         </is>
       </c>
       <c r="C206" t="inlineStr"/>
@@ -3757,7 +3757,7 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'NH3 to n2o [fraction of NH3]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base nh3 to n2o [fraction of NH3]')</t>
         </is>
       </c>
       <c r="C207" t="inlineStr"/>
@@ -3773,7 +3773,7 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>('Carbonizer base-A8', 'Carbon COD ratio [g C*g COD-1]')</t>
+          <t>('Carbonizer base-A8', 'Carbonizer base carbon COD ratio [g C*g COD-1]')</t>
         </is>
       </c>
       <c r="C208" t="inlineStr"/>
@@ -3789,7 +3789,7 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>('Pollution control device-A9', 'O2 sensor cost pcd [USD]')</t>
+          <t>('Pollution control device-A9', 'Pollution control device o2 sensor cost pcd [USD]')</t>
         </is>
       </c>
       <c r="C209" t="inlineStr"/>
@@ -3805,7 +3805,7 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>('Pollution control device-A9', 'Thermocouple cost cb pcd [USD]')</t>
+          <t>('Pollution control device-A9', 'Pollution control device thermocouple cost cb pcd [USD]')</t>
         </is>
       </c>
       <c r="C210" t="inlineStr"/>
@@ -3821,7 +3821,7 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>('Pollution control device-A9', 'Thermistor cost cb pcd [USD]')</t>
+          <t>('Pollution control device-A9', 'Pollution control device thermistor cost cb pcd [USD]')</t>
         </is>
       </c>
       <c r="C211" t="inlineStr"/>
@@ -3837,7 +3837,7 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>('Pollution control device-A9', 'Input auger pcd [USD]')</t>
+          <t>('Pollution control device-A9', 'Pollution control device input auger pcd [USD]')</t>
         </is>
       </c>
       <c r="C212" t="inlineStr"/>
@@ -3853,7 +3853,7 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>('Pollution control device-A9', 'Input auger motor pcd [USD]')</t>
+          <t>('Pollution control device-A9', 'Pollution control device input auger motor pcd [USD]')</t>
         </is>
       </c>
       <c r="C213" t="inlineStr"/>
@@ -3869,7 +3869,7 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>('Pollution control device-A9', 'Catylist pcd [USD]')</t>
+          <t>('Pollution control device-A9', 'Pollution control device catylist pcd [USD]')</t>
         </is>
       </c>
       <c r="C214" t="inlineStr"/>
@@ -3885,7 +3885,7 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>('Pollution control device-A9', 'Catalyst access door pcd [USD]')</t>
+          <t>('Pollution control device-A9', 'Pollution control device catalyst access door pcd [USD]')</t>
         </is>
       </c>
       <c r="C215" t="inlineStr"/>
@@ -3901,7 +3901,7 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>('Pollution control device-A9', 'Feedstock staging bin pcd [USD]')</t>
+          <t>('Pollution control device-A9', 'Pollution control device feedstock staging bin pcd [USD]')</t>
         </is>
       </c>
       <c r="C216" t="inlineStr"/>
@@ -3917,7 +3917,7 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>('Pollution control device-A9', 'Temperature limit switch pcd [USD]')</t>
+          <t>('Pollution control device-A9', 'Pollution control device temperature limit switch pcd [USD]')</t>
         </is>
       </c>
       <c r="C217" t="inlineStr"/>
@@ -3933,7 +3933,7 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>('Pollution control device-A9', 'Airlock pcd [USD]')</t>
+          <t>('Pollution control device-A9', 'Pollution control device airlock pcd [USD]')</t>
         </is>
       </c>
       <c r="C218" t="inlineStr"/>
@@ -3949,7 +3949,7 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>('Pollution control device-A9', 'Steel cost [USD/kg]')</t>
+          <t>('Pollution control device-A9', 'Pollution control device steel cost [USD/kg]')</t>
         </is>
       </c>
       <c r="C219" t="inlineStr"/>
@@ -3965,7 +3965,7 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>('Pollution control device-A9', 'Stainless steel cost [USD/kg]')</t>
+          <t>('Pollution control device-A9', 'Pollution control device stainless steel cost [USD/kg]')</t>
         </is>
       </c>
       <c r="C220" t="inlineStr"/>
@@ -3981,7 +3981,7 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>('Pollution control device-A9', 'Service team replacecatalyst pcd [min / corrective maintenance]')</t>
+          <t>('Pollution control device-A9', 'Pollution control device service team replacecatalyst pcd [min / corrective maintenance]')</t>
         </is>
       </c>
       <c r="C221" t="inlineStr"/>
@@ -3997,7 +3997,7 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>('Pollution control device-A9', 'Service team replacebrick pcd [min / corrective maintenance]')</t>
+          <t>('Pollution control device-A9', 'Pollution control device service team replacebrick pcd [min / corrective maintenance]')</t>
         </is>
       </c>
       <c r="C222" t="inlineStr"/>
@@ -4013,7 +4013,7 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>('Pollution control device-A9', 'Service team replaceo2sensor pcd [min / corrective maintenance]')</t>
+          <t>('Pollution control device-A9', 'Pollution control device service team replaceo2sensor pcd [min / corrective maintenance]')</t>
         </is>
       </c>
       <c r="C223" t="inlineStr"/>
@@ -4029,7 +4029,7 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>('Pollution control device-A9', 'Service team adjustdoor pcd [min / month]')</t>
+          <t>('Pollution control device-A9', 'Pollution control device service team adjustdoor pcd [min / month]')</t>
         </is>
       </c>
       <c r="C224" t="inlineStr"/>
@@ -4045,7 +4045,7 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>('Pollution control device-A9', 'Thermocouple lifetime cb 2pcd [y]')</t>
+          <t>('Pollution control device-A9', 'Pollution control device thermocouple lifetime cb 2pcd [y]')</t>
         </is>
       </c>
       <c r="C225" t="inlineStr"/>
@@ -4061,7 +4061,7 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>('Pollution control device-A9', 'Frequency corrective maintenance [y / occurance]')</t>
+          <t>('Pollution control device-A9', 'Pollution control device frequency corrective maintenance [y / occurance]')</t>
         </is>
       </c>
       <c r="C226" t="inlineStr"/>
@@ -4077,7 +4077,7 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>('Pollution control device-A9', 'Catalyst temp [C]')</t>
+          <t>('Pollution control device-A9', 'Pollution control device catalyst temp [C]')</t>
         </is>
       </c>
       <c r="C227" t="inlineStr"/>
@@ -6709,7 +6709,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>('Grinder-B10', 'Grinder [usd]')</t>
+          <t>('Grinder-B10', 'Grinder grinder [usd]')</t>
         </is>
       </c>
       <c r="C2" t="inlineStr"/>
@@ -6725,7 +6725,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>('Grinder-B10', 'Grinder steel [kg]')</t>
+          <t>('Grinder-B10', 'Grinder grinder steel [kg]')</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
@@ -6741,7 +6741,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>('Grinder-B10', 'Grinder electricity [kwh/kg]')</t>
+          <t>('Grinder-B10', 'Grinder grinder electricity [kwh/kg]')</t>
         </is>
       </c>
       <c r="C4" t="inlineStr"/>
@@ -6757,7 +6757,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Energy required to dry sludge [MJ/kg water]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base energy required to dry sludge [MJ/kg water]')</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
@@ -6773,7 +6773,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Dry feces heat of combustion [MJ/kg dry]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base dry feces heat of combustion [MJ/kg dry]')</t>
         </is>
       </c>
       <c r="C6" t="inlineStr"/>
@@ -6789,7 +6789,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Pyrolysis pot cost cb [USD]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base pyrolysis pot cost cb [USD]')</t>
         </is>
       </c>
       <c r="C7" t="inlineStr"/>
@@ -6805,7 +6805,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Char auger motor cost cb [USD]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base char auger motor cost cb [USD]')</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
@@ -6821,7 +6821,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Fuel auger motor cost cb [USD]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base fuel auger motor cost cb [USD]')</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
@@ -6837,7 +6837,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Primary air blower cost cb [USD]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base primary air blower cost cb [USD]')</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
@@ -6853,7 +6853,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Thermocouple cost cb pcd [USD]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base thermocouple cost cb pcd [USD]')</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
@@ -6869,7 +6869,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Thermistor cost cb pcd [USD]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base thermistor cost cb pcd [USD]')</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
@@ -6885,7 +6885,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Forced air fan cost cb [USD]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base forced air fan cost cb [USD]')</t>
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
@@ -6901,7 +6901,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Airlock motor cost cb [USD]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base airlock motor cost cb [USD]')</t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
@@ -6917,7 +6917,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Inducer fan cost cb [USD]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base inducer fan cost cb [USD]')</t>
         </is>
       </c>
       <c r="C15" t="inlineStr"/>
@@ -6933,7 +6933,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Biochar collection box cost cb [USD]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base biochar collection box cost cb [USD]')</t>
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
@@ -6949,7 +6949,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Chain guards cost cb [USD]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base chain guards cost cb [USD]')</t>
         </is>
       </c>
       <c r="C17" t="inlineStr"/>
@@ -6965,7 +6965,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Door cost cb [USD]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base door cost cb [USD]')</t>
         </is>
       </c>
       <c r="C18" t="inlineStr"/>
@@ -6981,7 +6981,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Agitator cost cb [USD]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base agitator cost cb [USD]')</t>
         </is>
       </c>
       <c r="C19" t="inlineStr"/>
@@ -6997,7 +6997,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Combusion chamber cost cb [USD]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base combusion chamber cost cb [USD]')</t>
         </is>
       </c>
       <c r="C20" t="inlineStr"/>
@@ -7013,7 +7013,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Sprayer cost cb [USD]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base sprayer cost cb [USD]')</t>
         </is>
       </c>
       <c r="C21" t="inlineStr"/>
@@ -7029,7 +7029,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Vent cost cb [USD]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base vent cost cb [USD]')</t>
         </is>
       </c>
       <c r="C22" t="inlineStr"/>
@@ -7045,7 +7045,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'SO2 emissions [mg/Nm3]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base so2 emissions [mg/Nm3]')</t>
         </is>
       </c>
       <c r="C23" t="inlineStr"/>
@@ -7061,7 +7061,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'CO emissions [mg/Nm3]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base CO emissions [mg/Nm3]')</t>
         </is>
       </c>
       <c r="C24" t="inlineStr"/>
@@ -7077,7 +7077,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Hg emissions [mg/Nm3]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base hg emissions [mg/Nm3]')</t>
         </is>
       </c>
       <c r="C25" t="inlineStr"/>
@@ -7093,7 +7093,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Cd emissions [mg/Nm3]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base cd emissions [mg/Nm3]')</t>
         </is>
       </c>
       <c r="C26" t="inlineStr"/>
@@ -7109,7 +7109,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'As emissions [mg/Nm3]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base as emissions [mg/Nm3]')</t>
         </is>
       </c>
       <c r="C27" t="inlineStr"/>
@@ -7125,7 +7125,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Dioxin furans emissions [ng/Nm3]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base dioxin furans emissions [ng/Nm3]')</t>
         </is>
       </c>
       <c r="C28" t="inlineStr"/>
@@ -7141,7 +7141,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Cb n2o emissions [% of total N]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base cb n2o emissions [% of total N]')</t>
         </is>
       </c>
       <c r="C29" t="inlineStr"/>
@@ -7157,7 +7157,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Steel cost [USD/kg]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base steel cost [USD/kg]')</t>
         </is>
       </c>
       <c r="C30" t="inlineStr"/>
@@ -7173,7 +7173,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Stainless steel cost [USD/kg]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base stainless steel cost [USD/kg]')</t>
         </is>
       </c>
       <c r="C31" t="inlineStr"/>
@@ -7189,7 +7189,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Primary air blower lifetime cb [y]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base primary air blower lifetime cb [y]')</t>
         </is>
       </c>
       <c r="C32" t="inlineStr"/>
@@ -7205,7 +7205,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Thermocouple lifetime cb 2pcd [y]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base thermocouple lifetime cb 2pcd [y]')</t>
         </is>
       </c>
       <c r="C33" t="inlineStr"/>
@@ -7221,7 +7221,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Forced air fan lifetime cb [y]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base forced air fan lifetime cb [y]')</t>
         </is>
       </c>
       <c r="C34" t="inlineStr"/>
@@ -7237,7 +7237,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Airlock motor lifetime cb [y]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base airlock motor lifetime cb [y]')</t>
         </is>
       </c>
       <c r="C35" t="inlineStr"/>
@@ -7253,7 +7253,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Inducer fan lifetime cb [y]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base inducer fan lifetime cb [y]')</t>
         </is>
       </c>
       <c r="C36" t="inlineStr"/>
@@ -7269,7 +7269,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Service team replacegasket cb [min / corrective maintenance]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base service team replacegasket cb [min / corrective maintenance]')</t>
         </is>
       </c>
       <c r="C37" t="inlineStr"/>
@@ -7285,7 +7285,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Service team replacedoor cb [min / corrective maintenance]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base service team replacedoor cb [min / corrective maintenance]')</t>
         </is>
       </c>
       <c r="C38" t="inlineStr"/>
@@ -7301,7 +7301,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Service team replacechain cb [min / corrective maintenance]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base service team replacechain cb [min / corrective maintenance]')</t>
         </is>
       </c>
       <c r="C39" t="inlineStr"/>
@@ -7317,7 +7317,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Service team changefirepot cb [min / corrective maintenance]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base service team changefirepot cb [min / corrective maintenance]')</t>
         </is>
       </c>
       <c r="C40" t="inlineStr"/>
@@ -7333,7 +7333,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Service team replacecharaugers cb [min / corrective maintenance]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base service team replacecharaugers cb [min / corrective maintenance]')</t>
         </is>
       </c>
       <c r="C41" t="inlineStr"/>
@@ -7349,7 +7349,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Service team replacecatalyst pcd [min / corrective maintenance]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base service team replacecatalyst pcd [min / corrective maintenance]')</t>
         </is>
       </c>
       <c r="C42" t="inlineStr"/>
@@ -7365,7 +7365,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Service team replacebrick pcd [min / corrective maintenance]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base service team replacebrick pcd [min / corrective maintenance]')</t>
         </is>
       </c>
       <c r="C43" t="inlineStr"/>
@@ -7381,7 +7381,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Service team replacefuelauger pcd [min / corrective maintenance]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base service team replacefuelauger pcd [min / corrective maintenance]')</t>
         </is>
       </c>
       <c r="C44" t="inlineStr"/>
@@ -7397,7 +7397,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Service team replacewaterpump hhx [min / corrective maintenance]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base service team replacewaterpump hhx [min / corrective maintenance]')</t>
         </is>
       </c>
       <c r="C45" t="inlineStr"/>
@@ -7413,7 +7413,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Service team purgewaterloop hhx [min / corrective maintenance]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base service team purgewaterloop hhx [min / corrective maintenance]')</t>
         </is>
       </c>
       <c r="C46" t="inlineStr"/>
@@ -7429,7 +7429,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Service team replacecharmotor cb [min / corrective maintenance]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base service team replacecharmotor cb [min / corrective maintenance]')</t>
         </is>
       </c>
       <c r="C47" t="inlineStr"/>
@@ -7445,7 +7445,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Service team replacefuelmotor cb [min / corrective maintenance]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base service team replacefuelmotor cb [min / corrective maintenance]')</t>
         </is>
       </c>
       <c r="C48" t="inlineStr"/>
@@ -7461,7 +7461,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Service team replaceblower cb [min / corrective maintenance]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base service team replaceblower cb [min / corrective maintenance]')</t>
         </is>
       </c>
       <c r="C49" t="inlineStr"/>
@@ -7477,7 +7477,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Service team replacefan cb [min / corrective maintenance]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base service team replacefan cb [min / corrective maintenance]')</t>
         </is>
       </c>
       <c r="C50" t="inlineStr"/>
@@ -7493,7 +7493,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Service team replaceo2sensor pcd [min / corrective maintenance]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base service team replaceo2sensor pcd [min / corrective maintenance]')</t>
         </is>
       </c>
       <c r="C51" t="inlineStr"/>
@@ -7509,7 +7509,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Service team replacepaddleswitch cb [min / corrective maintenance]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base service team replacepaddleswitch cb [min / corrective maintenance]')</t>
         </is>
       </c>
       <c r="C52" t="inlineStr"/>
@@ -7525,7 +7525,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Service team replaceairlock cb [min / corrective maintenance]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base service team replaceairlock cb [min / corrective maintenance]')</t>
         </is>
       </c>
       <c r="C53" t="inlineStr"/>
@@ -7541,7 +7541,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Service team greasebearing cb [min / month]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base service team greasebearing cb [min / month]')</t>
         </is>
       </c>
       <c r="C54" t="inlineStr"/>
@@ -7557,7 +7557,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Service team tighten cb [min / month]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base service team tighten cb [min / month]')</t>
         </is>
       </c>
       <c r="C55" t="inlineStr"/>
@@ -7573,7 +7573,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Service team adjustdoor cb [min / month]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base service team adjustdoor cb [min / month]')</t>
         </is>
       </c>
       <c r="C56" t="inlineStr"/>
@@ -7589,7 +7589,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Service team adjustdoor pcd [min / month]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base service team adjustdoor pcd [min / month]')</t>
         </is>
       </c>
       <c r="C57" t="inlineStr"/>
@@ -7605,7 +7605,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Service team adjustdoor hhx [min / month]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base service team adjustdoor hhx [min / month]')</t>
         </is>
       </c>
       <c r="C58" t="inlineStr"/>
@@ -7621,7 +7621,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Frequency corrective maintenance [y / occurance]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base frequency corrective maintenance [y / occurance]')</t>
         </is>
       </c>
       <c r="C59" t="inlineStr"/>
@@ -7637,7 +7637,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Biochar calorific value [MJ/kg dry]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base biochar calorific value [MJ/kg dry]')</t>
         </is>
       </c>
       <c r="C60" t="inlineStr"/>
@@ -7653,7 +7653,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Pyrolysis temp [C]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base pyrolysis temp [C]')</t>
         </is>
       </c>
       <c r="C61" t="inlineStr"/>
@@ -7669,7 +7669,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Pyrolysis C loss [fraction of total C]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base pyrolysis C loss [fraction of total C]')</t>
         </is>
       </c>
       <c r="C62" t="inlineStr"/>
@@ -7685,7 +7685,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Pyrolysis N loss [fraction of total N]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base pyrolysis N loss [fraction of total N]')</t>
         </is>
       </c>
       <c r="C63" t="inlineStr"/>
@@ -7701,7 +7701,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Pyrolysis K loss [fraction of total K]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base pyrolysis K loss [fraction of total K]')</t>
         </is>
       </c>
       <c r="C64" t="inlineStr"/>
@@ -7717,7 +7717,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Pyrolysis P loss [fraction of total P]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base pyrolysis P loss [fraction of total P]')</t>
         </is>
       </c>
       <c r="C65" t="inlineStr"/>
@@ -7733,7 +7733,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'N to NH3 [fraction of N]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer Base N to NH3 [fraction of N]')</t>
         </is>
       </c>
       <c r="C66" t="inlineStr"/>
@@ -7749,7 +7749,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'N to HCNO [fraction of N]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base N to HCNO [fraction of N]')</t>
         </is>
       </c>
       <c r="C67" t="inlineStr"/>
@@ -7765,7 +7765,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'HCNO to NH3 [fraction of HCNO]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer Base HCNO to NH3 [fraction of HCNO]')</t>
         </is>
       </c>
       <c r="C68" t="inlineStr"/>
@@ -7781,7 +7781,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'NH3 to n2o [fraction of NH3]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base nh3 to n2o [fraction of NH3]')</t>
         </is>
       </c>
       <c r="C69" t="inlineStr"/>
@@ -7797,7 +7797,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>('Carbonizer base-B11', 'Carbon COD ratio [g C*g COD-1]')</t>
+          <t>('Carbonizer base-B11', 'Carbonizer base carbon COD ratio [g C*g COD-1]')</t>
         </is>
       </c>
       <c r="C70" t="inlineStr"/>
@@ -7813,7 +7813,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>('Pollution control device-B12', 'O2 sensor cost pcd [USD]')</t>
+          <t>('Pollution control device-B12', 'Pollution control device o2 sensor cost pcd [USD]')</t>
         </is>
       </c>
       <c r="C71" t="inlineStr"/>
@@ -7829,7 +7829,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>('Pollution control device-B12', 'Thermocouple cost cb pcd [USD]')</t>
+          <t>('Pollution control device-B12', 'Pollution control device thermocouple cost cb pcd [USD]')</t>
         </is>
       </c>
       <c r="C72" t="inlineStr"/>
@@ -7845,7 +7845,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>('Pollution control device-B12', 'Thermistor cost cb pcd [USD]')</t>
+          <t>('Pollution control device-B12', 'Pollution control device thermistor cost cb pcd [USD]')</t>
         </is>
       </c>
       <c r="C73" t="inlineStr"/>
@@ -7861,7 +7861,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>('Pollution control device-B12', 'Input auger pcd [USD]')</t>
+          <t>('Pollution control device-B12', 'Pollution control device input auger pcd [USD]')</t>
         </is>
       </c>
       <c r="C74" t="inlineStr"/>
@@ -7877,7 +7877,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>('Pollution control device-B12', 'Input auger motor pcd [USD]')</t>
+          <t>('Pollution control device-B12', 'Pollution control device input auger motor pcd [USD]')</t>
         </is>
       </c>
       <c r="C75" t="inlineStr"/>
@@ -7893,7 +7893,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>('Pollution control device-B12', 'Catylist pcd [USD]')</t>
+          <t>('Pollution control device-B12', 'Pollution control device catylist pcd [USD]')</t>
         </is>
       </c>
       <c r="C76" t="inlineStr"/>
@@ -7909,7 +7909,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>('Pollution control device-B12', 'Catalyst access door pcd [USD]')</t>
+          <t>('Pollution control device-B12', 'Pollution control device catalyst access door pcd [USD]')</t>
         </is>
       </c>
       <c r="C77" t="inlineStr"/>
@@ -7925,7 +7925,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>('Pollution control device-B12', 'Feedstock staging bin pcd [USD]')</t>
+          <t>('Pollution control device-B12', 'Pollution control device feedstock staging bin pcd [USD]')</t>
         </is>
       </c>
       <c r="C78" t="inlineStr"/>
@@ -7941,7 +7941,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>('Pollution control device-B12', 'Temperature limit switch pcd [USD]')</t>
+          <t>('Pollution control device-B12', 'Pollution control device temperature limit switch pcd [USD]')</t>
         </is>
       </c>
       <c r="C79" t="inlineStr"/>
@@ -7957,7 +7957,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>('Pollution control device-B12', 'Airlock pcd [USD]')</t>
+          <t>('Pollution control device-B12', 'Pollution control device airlock pcd [USD]')</t>
         </is>
       </c>
       <c r="C80" t="inlineStr"/>
@@ -7973,7 +7973,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>('Pollution control device-B12', 'Steel cost [USD/kg]')</t>
+          <t>('Pollution control device-B12', 'Pollution control device steel cost [USD/kg]')</t>
         </is>
       </c>
       <c r="C81" t="inlineStr"/>
@@ -7989,7 +7989,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>('Pollution control device-B12', 'Stainless steel cost [USD/kg]')</t>
+          <t>('Pollution control device-B12', 'Pollution control device stainless steel cost [USD/kg]')</t>
         </is>
       </c>
       <c r="C82" t="inlineStr"/>
@@ -8005,7 +8005,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>('Pollution control device-B12', 'Service team replacecatalyst pcd [min / corrective maintenance]')</t>
+          <t>('Pollution control device-B12', 'Pollution control device service team replacecatalyst pcd [min / corrective maintenance]')</t>
         </is>
       </c>
       <c r="C83" t="inlineStr"/>
@@ -8021,7 +8021,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>('Pollution control device-B12', 'Service team replacebrick pcd [min / corrective maintenance]')</t>
+          <t>('Pollution control device-B12', 'Pollution control device service team replacebrick pcd [min / corrective maintenance]')</t>
         </is>
       </c>
       <c r="C84" t="inlineStr"/>
@@ -8037,7 +8037,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>('Pollution control device-B12', 'Service team replaceo2sensor pcd [min / corrective maintenance]')</t>
+          <t>('Pollution control device-B12', 'Pollution control device service team replaceo2sensor pcd [min / corrective maintenance]')</t>
         </is>
       </c>
       <c r="C85" t="inlineStr"/>
@@ -8053,7 +8053,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>('Pollution control device-B12', 'Service team adjustdoor pcd [min / month]')</t>
+          <t>('Pollution control device-B12', 'Pollution control device service team adjustdoor pcd [min / month]')</t>
         </is>
       </c>
       <c r="C86" t="inlineStr"/>
@@ -8069,7 +8069,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>('Pollution control device-B12', 'Thermocouple lifetime cb 2pcd [y]')</t>
+          <t>('Pollution control device-B12', 'Pollution control device thermocouple lifetime cb 2pcd [y]')</t>
         </is>
       </c>
       <c r="C87" t="inlineStr"/>
@@ -8085,7 +8085,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>('Pollution control device-B12', 'Frequency corrective maintenance [y / occurance]')</t>
+          <t>('Pollution control device-B12', 'Pollution control device frequency corrective maintenance [y / occurance]')</t>
         </is>
       </c>
       <c r="C88" t="inlineStr"/>
@@ -8101,7 +8101,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>('Pollution control device-B12', 'Catalyst temp [C]')</t>
+          <t>('Pollution control device-B12', 'Pollution control device catalyst temp [C]')</t>
         </is>
       </c>
       <c r="C89" t="inlineStr"/>
@@ -8117,7 +8117,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>('Oil heat exchanger-B13', 'Orc cost [USD]')</t>
+          <t>('Oil heat exchanger-B13', 'Oil heat exchanger orc cost [USD]')</t>
         </is>
       </c>
       <c r="C90" t="inlineStr"/>
@@ -8133,7 +8133,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>('Oil heat exchanger-B13', 'Oil pump power [kW]')</t>
+          <t>('Oil heat exchanger-B13', 'Oil heat exchanger oil pump power [kW]')</t>
         </is>
       </c>
       <c r="C91" t="inlineStr"/>
@@ -8149,7 +8149,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>('Oil heat exchanger-B13', 'Oil electrical energy generated [kW]')</t>
+          <t>('Oil heat exchanger-B13', 'Oil heat exchanger oil electrical energy generated [kW]')</t>
         </is>
       </c>
       <c r="C92" t="inlineStr"/>
@@ -8165,7 +8165,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>('Oil heat exchanger-B13', 'Oil flowrate [L/min]')</t>
+          <t>('Oil heat exchanger-B13', 'Oil heat exchanger oil flowrate [L/min]')</t>
         </is>
       </c>
       <c r="C93" t="inlineStr"/>
@@ -8181,7 +8181,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>('Oil heat exchanger-B13', 'Ohx temp [C]')</t>
+          <t>('Oil heat exchanger-B13', 'Oil heat exchanger ohx temp [C]')</t>
         </is>
       </c>
       <c r="C94" t="inlineStr"/>
@@ -8197,7 +8197,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>('Oil heat exchanger-B13', 'Oil temp in [C]')</t>
+          <t>('Oil heat exchanger-B13', 'Oil heat exchanger oil temp in [C]')</t>
         </is>
       </c>
       <c r="C95" t="inlineStr"/>
@@ -8213,7 +8213,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>('Oil heat exchanger-B13', 'Oil temp out [C]')</t>
+          <t>('Oil heat exchanger-B13', 'Oil heat exchanger oil temp out [C]')</t>
         </is>
       </c>
       <c r="C96" t="inlineStr"/>
@@ -8229,7 +8229,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>('Oil heat exchanger-B13', 'Amb temp [C]')</t>
+          <t>('Oil heat exchanger-B13', 'Oil heat exchanger amb temp [C]')</t>
         </is>
       </c>
       <c r="C97" t="inlineStr"/>
@@ -8245,7 +8245,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-B14', 'Heat exchanger hydronic steel [kg]')</t>
+          <t>('Hydronic heat exchanger-B14', 'Hydronic heat exchanger heat exchanger hydronic steel [kg]')</t>
         </is>
       </c>
       <c r="C98" t="inlineStr"/>
@@ -8261,7 +8261,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-B14', 'Heat exchanger hydronic stainless [kg]')</t>
+          <t>('Hydronic heat exchanger-B14', 'Hydronic heat exchanger heat exchanger hydronic stainless [kg]')</t>
         </is>
       </c>
       <c r="C99" t="inlineStr"/>
@@ -8277,7 +8277,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-B14', 'Water pump power [kW]')</t>
+          <t>('Hydronic heat exchanger-B14', 'Hydronic heat exchanger water pump power [kW]')</t>
         </is>
       </c>
       <c r="C100" t="inlineStr"/>
@@ -8293,7 +8293,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-B14', 'Hhx inducer fan power [kW]')</t>
+          <t>('Hydronic heat exchanger-B14', 'Hydronic heat exchanger hhx inducer fan power [kW]')</t>
         </is>
       </c>
       <c r="C101" t="inlineStr"/>
@@ -8309,7 +8309,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-B14', 'Hhx stack [USD]')</t>
+          <t>('Hydronic heat exchanger-B14', 'Hydronic heat exchanger hhx stack [USD]')</t>
         </is>
       </c>
       <c r="C102" t="inlineStr"/>
@@ -8325,7 +8325,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-B14', 'Hhx stack thermocouple [USD]')</t>
+          <t>('Hydronic heat exchanger-B14', 'Hydronic heat exchanger hhx stack thermocouple [USD]')</t>
         </is>
       </c>
       <c r="C103" t="inlineStr"/>
@@ -8341,7 +8341,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-B14', 'Hhx oxygen sensor [USD]')</t>
+          <t>('Hydronic heat exchanger-B14', 'Hydronic heat exchanger hhx oxygen sensor [USD]')</t>
         </is>
       </c>
       <c r="C104" t="inlineStr"/>
@@ -8357,7 +8357,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-B14', 'Hhx inducer fan [USD]')</t>
+          <t>('Hydronic heat exchanger-B14', 'Hydronic heat exchanger hhx inducer fan [USD]')</t>
         </is>
       </c>
       <c r="C105" t="inlineStr"/>
@@ -8373,7 +8373,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-B14', 'Hhx flow meter [USD]')</t>
+          <t>('Hydronic heat exchanger-B14', 'Hydronic heat exchanger hhx flow meter [USD]')</t>
         </is>
       </c>
       <c r="C106" t="inlineStr"/>
@@ -8389,7 +8389,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-B14', 'Hhx pump [USD]')</t>
+          <t>('Hydronic heat exchanger-B14', 'Hydronic heat exchanger hhx pump [USD]')</t>
         </is>
       </c>
       <c r="C107" t="inlineStr"/>
@@ -8405,7 +8405,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-B14', 'Hhx water in thermistor [USD]')</t>
+          <t>('Hydronic heat exchanger-B14', 'Hydronic heat exchanger hhx water in thermistor [USD]')</t>
         </is>
       </c>
       <c r="C108" t="inlineStr"/>
@@ -8421,7 +8421,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-B14', 'Hhx water out thermistor [USD]')</t>
+          <t>('Hydronic heat exchanger-B14', 'Hydronic heat exchanger hhx water out thermistor [USD]')</t>
         </is>
       </c>
       <c r="C109" t="inlineStr"/>
@@ -8437,7 +8437,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-B14', 'Hhx load tank [USD]')</t>
+          <t>('Hydronic heat exchanger-B14', 'Hydronic heat exchanger hhx load tank [USD]')</t>
         </is>
       </c>
       <c r="C110" t="inlineStr"/>
@@ -8453,7 +8453,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-B14', 'Hhx expansion tank [USD]')</t>
+          <t>('Hydronic heat exchanger-B14', 'Hydronic heat exchanger hhx expansion tank [USD]')</t>
         </is>
       </c>
       <c r="C111" t="inlineStr"/>
@@ -8469,7 +8469,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-B14', 'Hhx heat exchanger [USD]')</t>
+          <t>('Hydronic heat exchanger-B14', 'Hydronic heat exchanger hhx heat exchanger [USD]')</t>
         </is>
       </c>
       <c r="C112" t="inlineStr"/>
@@ -8485,7 +8485,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-B14', 'Hhx values [USD]')</t>
+          <t>('Hydronic heat exchanger-B14', 'Hydronic heat exchanger hhx values [USD]')</t>
         </is>
       </c>
       <c r="C113" t="inlineStr"/>
@@ -8501,7 +8501,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-B14', 'Hhx thermal well [USD]')</t>
+          <t>('Hydronic heat exchanger-B14', 'Hydronic heat exchanger hhx thermal well [USD]')</t>
         </is>
       </c>
       <c r="C114" t="inlineStr"/>
@@ -8517,7 +8517,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-B14', 'Hhx hot water tank [USD]')</t>
+          <t>('Hydronic heat exchanger-B14', 'Hydronic heat exchanger hhx hot water tank [USD]')</t>
         </is>
       </c>
       <c r="C115" t="inlineStr"/>
@@ -8533,7 +8533,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-B14', 'Hhx overflow tank [USD]')</t>
+          <t>('Hydronic heat exchanger-B14', 'Hydronic heat exchanger hhx overflow tank [USD]')</t>
         </is>
       </c>
       <c r="C116" t="inlineStr"/>
@@ -8549,7 +8549,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-B14', 'Steel cost [USD/kg]')</t>
+          <t>('Hydronic heat exchanger-B14', 'Hydronic heat exchanger steel cost [USD/kg]')</t>
         </is>
       </c>
       <c r="C117" t="inlineStr"/>
@@ -8565,7 +8565,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-B14', 'Stainless steel cost [USD/kg]')</t>
+          <t>('Hydronic heat exchanger-B14', 'Hydronic heat exchanger stainless steel cost [USD/kg]')</t>
         </is>
       </c>
       <c r="C118" t="inlineStr"/>
@@ -8581,7 +8581,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-B14', 'Frequency corrective maintenance [y / occurance]')</t>
+          <t>('Hydronic heat exchanger-B14', 'Hydronic heat exchanger frequency corrective maintenance [y / occurance]')</t>
         </is>
       </c>
       <c r="C119" t="inlineStr"/>
@@ -8597,7 +8597,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-B14', 'Service team adjustdoor hhx [min / month]')</t>
+          <t>('Hydronic heat exchanger-B14', 'Hydronic heat exchanger service team adjustdoor hhx [min / month]')</t>
         </is>
       </c>
       <c r="C120" t="inlineStr"/>
@@ -8613,7 +8613,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-B14', 'Service team replacewaterpump hhx [min / corrective maintenance]')</t>
+          <t>('Hydronic heat exchanger-B14', 'Hydronic heat exchanger service team replacewaterpump hhx [min / corrective maintenance]')</t>
         </is>
       </c>
       <c r="C121" t="inlineStr"/>
@@ -8629,7 +8629,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-B14', 'Service team purgewaterloop hhx [min / corrective maintenance]')</t>
+          <t>('Hydronic heat exchanger-B14', 'Hydronic heat exchanger service team purgewaterloop hhx [min / corrective maintenance]')</t>
         </is>
       </c>
       <c r="C122" t="inlineStr"/>
@@ -8645,7 +8645,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-B14', 'Hhx temp [C]')</t>
+          <t>('Hydronic heat exchanger-B14', 'Hydronic heat exchanger hhx temp [C]')</t>
         </is>
       </c>
       <c r="C123" t="inlineStr"/>
@@ -8661,7 +8661,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-B14', 'Water flowrate [L/min]')</t>
+          <t>('Hydronic heat exchanger-B14', 'Hydronic heat exchanger water flowrate [L/min]')</t>
         </is>
       </c>
       <c r="C124" t="inlineStr"/>
@@ -8677,7 +8677,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-B14', 'Water out temp [C]')</t>
+          <t>('Hydronic heat exchanger-B14', 'Hydronic heat exchanger water out temp [C]')</t>
         </is>
       </c>
       <c r="C125" t="inlineStr"/>
@@ -8693,7 +8693,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-B14', 'Water in temp [C]')</t>
+          <t>('Hydronic heat exchanger-B14', 'Hydronic heat exchanger water in temp [C]')</t>
         </is>
       </c>
       <c r="C126" t="inlineStr"/>
@@ -8709,7 +8709,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>('Hydronic heat exchanger-B14', 'Ambient temp [C]')</t>
+          <t>('Hydronic heat exchanger-B14', 'Hydronic heat exchanger ambient temp [C]')</t>
         </is>
       </c>
       <c r="C127" t="inlineStr"/>
@@ -8725,7 +8725,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>('HHXdryer-B15', 'Drying energy demand [kW]')</t>
+          <t>('HHXdryer-B15', 'HHXdryer drying energy demand [kW]')</t>
         </is>
       </c>
       <c r="C128" t="inlineStr"/>
@@ -8741,7 +8741,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>('HHXdryer-B15', 'Drying co2 emissions [% of total C]')</t>
+          <t>('HHXdryer-B15', 'HHXdryer drying co2 emissions [% of total C]')</t>
         </is>
       </c>
       <c r="C129" t="inlineStr"/>
@@ -8757,7 +8757,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>('HHXdryer-B15', 'Drying ch4 emissions [% of total C]')</t>
+          <t>('HHXdryer-B15', 'HHXdryer drying ch4 emissions [% of total C]')</t>
         </is>
       </c>
       <c r="C130" t="inlineStr"/>
@@ -8773,7 +8773,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>('HHXdryer-B15', 'Drying nh3 emissions [% of total N]')</t>
+          <t>('HHXdryer-B15', 'HHXdryer drying nh3 emissions [% of total N]')</t>
         </is>
       </c>
       <c r="C131" t="inlineStr"/>
@@ -8789,7 +8789,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>('HHXdryer-B15', 'NH3 to n2o [% of NH3]')</t>
+          <t>('HHXdryer-B15', 'HHXdryer nh3 to n2o [% of NH3]')</t>
         </is>
       </c>
       <c r="C132" t="inlineStr"/>
@@ -8805,7 +8805,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>('HHXdryer-B15', 'Energy required to dry sludge [MJ/kg water]')</t>
+          <t>('HHXdryer-B15', 'HHXdryer energy required to dry sludge [MJ/kg water]')</t>
         </is>
       </c>
       <c r="C133" t="inlineStr"/>
@@ -8821,7 +8821,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>('HHXdryer-B15', 'Ambient temp [C]')</t>
+          <t>('HHXdryer-B15', 'HHXdryer ambient temp [C]')</t>
         </is>
       </c>
       <c r="C134" t="inlineStr"/>
@@ -8837,7 +8837,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>('HHXdryer-B15', 'Dryer heat transfer coeff [MJ / (h m2 K)]')</t>
+          <t>('HHXdryer-B15', 'HHXdryer dryer heat transfer coeff [MJ / (h m2 K)]')</t>
         </is>
       </c>
       <c r="C135" t="inlineStr"/>
@@ -8853,7 +8853,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>('HHXdryer-B15', 'Water out temp [C]')</t>
+          <t>('HHXdryer-B15', 'HHXdryer water out temp [C]')</t>
         </is>
       </c>
       <c r="C136" t="inlineStr"/>
@@ -8869,7 +8869,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>('HHXdryer-B15', 'Carbon COD ratio [g C*g COD-1]')</t>
+          <t>('HHXdryer-B15', 'HHXdryer carbon COD ratio [g C*g COD-1]')</t>
         </is>
       </c>
       <c r="C137" t="inlineStr"/>
@@ -8885,7 +8885,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'N prot [fraction]')</t>
+          <t>('Excretion-B1', 'Excretion N prot [fraction]')</t>
         </is>
       </c>
       <c r="C138" t="inlineStr"/>
@@ -8901,7 +8901,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'P prot v [fraction]')</t>
+          <t>('Excretion-B1', 'Excretion P prot v [fraction]')</t>
         </is>
       </c>
       <c r="C139" t="inlineStr"/>
@@ -8917,7 +8917,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'P prot a [fraction]')</t>
+          <t>('Excretion-B1', 'Excretion P prot a [fraction]')</t>
         </is>
       </c>
       <c r="C140" t="inlineStr"/>
@@ -8933,7 +8933,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'K cal [g K/1000 kcal]')</t>
+          <t>('Excretion-B1', 'Excretion K cal [g K/1000 kcal]')</t>
         </is>
       </c>
       <c r="C141" t="inlineStr"/>
@@ -8949,7 +8949,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'N exc [fraction of intake]')</t>
+          <t>('Excretion-B1', 'Excretion N exc [fraction of intake]')</t>
         </is>
       </c>
       <c r="C142" t="inlineStr"/>
@@ -8965,7 +8965,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'P exc [fraction of intake]')</t>
+          <t>('Excretion-B1', 'Excretion P exc [fraction of intake]')</t>
         </is>
       </c>
       <c r="C143" t="inlineStr"/>
@@ -8981,7 +8981,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'K exc [fraction of intake]')</t>
+          <t>('Excretion-B1', 'Excretion K exc [fraction of intake]')</t>
         </is>
       </c>
       <c r="C144" t="inlineStr"/>
@@ -8997,7 +8997,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'E exc [fraction of intake]')</t>
+          <t>('Excretion-B1', 'Excretion e exc [fraction of intake]')</t>
         </is>
       </c>
       <c r="C145" t="inlineStr"/>
@@ -9013,7 +9013,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'N ur [fraction of total]')</t>
+          <t>('Excretion-B1', 'Excretion N ur [fraction of total]')</t>
         </is>
       </c>
       <c r="C146" t="inlineStr"/>
@@ -9029,7 +9029,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'P ur [fraction of total]')</t>
+          <t>('Excretion-B1', 'Excretion P ur [fraction of total]')</t>
         </is>
       </c>
       <c r="C147" t="inlineStr"/>
@@ -9045,7 +9045,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'K ur [fraction of total]')</t>
+          <t>('Excretion-B1', 'Excretion K ur [fraction of total]')</t>
         </is>
       </c>
       <c r="C148" t="inlineStr"/>
@@ -9061,7 +9061,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'E fec [fraction of total]')</t>
+          <t>('Excretion-B1', 'Excretion e fec [fraction of total]')</t>
         </is>
       </c>
       <c r="C149" t="inlineStr"/>
@@ -9077,7 +9077,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'N ur NH3 [fraction of total N in urine]')</t>
+          <t>('Excretion-B1', 'Excretion N ur NH3 [fraction of total N in urine]')</t>
         </is>
       </c>
       <c r="C150" t="inlineStr"/>
@@ -9093,7 +9093,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'N fec NH3 [fraction of total N in feces]')</t>
+          <t>('Excretion-B1', 'Excretion N fec NH3 [fraction of total N in feces]')</t>
         </is>
       </c>
       <c r="C151" t="inlineStr"/>
@@ -9109,7 +9109,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'Ur exc [g/cap/d]')</t>
+          <t>('Excretion-B1', 'Excretion ur exc [g/cap/d]')</t>
         </is>
       </c>
       <c r="C152" t="inlineStr"/>
@@ -9125,7 +9125,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'Fec exc [g/cap/d]')</t>
+          <t>('Excretion-B1', 'Excretion fec exc [g/cap/d]')</t>
         </is>
       </c>
       <c r="C153" t="inlineStr"/>
@@ -9141,7 +9141,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'Ur moi [fraction]')</t>
+          <t>('Excretion-B1', 'Excretion ur moi [fraction]')</t>
         </is>
       </c>
       <c r="C154" t="inlineStr"/>
@@ -9157,7 +9157,7 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'Fec moi [fraction]')</t>
+          <t>('Excretion-B1', 'Excretion fec moi [fraction]')</t>
         </is>
       </c>
       <c r="C155" t="inlineStr"/>
@@ -9173,7 +9173,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'Mg ur [g Mg/cap/d]')</t>
+          <t>('Excretion-B1', 'Excretion mg ur [g Mg/cap/d]')</t>
         </is>
       </c>
       <c r="C156" t="inlineStr"/>
@@ -9189,7 +9189,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'Mg fec [g Mg/cap/d]')</t>
+          <t>('Excretion-B1', 'Excretion mg fec [g Mg/cap/d]')</t>
         </is>
       </c>
       <c r="C157" t="inlineStr"/>
@@ -9205,7 +9205,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'Ca ur [g Ca/cap/d]')</t>
+          <t>('Excretion-B1', 'Excretion ca ur [g Ca/cap/d]')</t>
         </is>
       </c>
       <c r="C158" t="inlineStr"/>
@@ -9221,7 +9221,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>('Excretion-B1', 'Ca fec [g Ca/cap/d]')</t>
+          <t>('Excretion-B1', 'Excretion ca fec [g Ca/cap/d]')</t>
         </is>
       </c>
       <c r="C159" t="inlineStr"/>
@@ -9381,7 +9381,7 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>('UDDT-B2', 'Toilet paper [kg/cap/hr]')</t>
+          <t>('UDDT-B2', 'UDDT toilet paper [kg/cap/hr]')</t>
         </is>
       </c>
       <c r="C169" t="inlineStr"/>
@@ -9397,7 +9397,7 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>('UDDT-B2', 'Flushing water [kg/cap/hr]')</t>
+          <t>('UDDT-B2', 'UDDT flushing water [kg/cap/hr]')</t>
         </is>
       </c>
       <c r="C170" t="inlineStr"/>
@@ -9413,7 +9413,7 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>('UDDT-B2', 'Cleansing water [kg/cap/hr]')</t>
+          <t>('UDDT-B2', 'UDDT cleansing water [kg/cap/hr]')</t>
         </is>
       </c>
       <c r="C171" t="inlineStr"/>
@@ -9429,7 +9429,7 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>('UDDT-B2', 'Desiccant V [m3/cap/hr]')</t>
+          <t>('UDDT-B2', 'UDDT desiccant V [m3/cap/hr]')</t>
         </is>
       </c>
       <c r="C172" t="inlineStr"/>
@@ -9445,7 +9445,7 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>('UDDT-B2', 'Desiccant rho [kg/m3]')</t>
+          <t>('UDDT-B2', 'UDDT desiccant rho [kg/m3]')</t>
         </is>
       </c>
       <c r="C173" t="inlineStr"/>
@@ -9461,7 +9461,7 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>('UDDT-B2', 'COD max decay [fraction of oxygen demand removal]')</t>
+          <t>('UDDT-B2', 'UDDT COD max decay [fraction of oxygen demand removal]')</t>
         </is>
       </c>
       <c r="C174" t="inlineStr"/>
@@ -9477,7 +9477,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>('UDDT-B2', 'N max decay [fraction of N removal after N leaching]')</t>
+          <t>('UDDT-B2', 'UDDT N max decay [fraction of N removal after N leaching]')</t>
         </is>
       </c>
       <c r="C175" t="inlineStr"/>
@@ -9493,7 +9493,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>('UDDT-B2', 'MCF aq [fraction of anaerobic conversion of degraded COD]')</t>
+          <t>('UDDT-B2', 'UDDT MCF aq [fraction of anaerobic conversion of degraded COD]')</t>
         </is>
       </c>
       <c r="C176" t="inlineStr"/>
@@ -9509,7 +9509,7 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>('UDDT-B2', 'N2O EF aq [fraction of N emitted as N2O]')</t>
+          <t>('UDDT-B2', 'UDDT n2o EF aq [fraction of N emitted as N2O]')</t>
         </is>
       </c>
       <c r="C177" t="inlineStr"/>
@@ -9525,7 +9525,7 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>('UDDT-B2', 'Collection period [d]')</t>
+          <t>('UDDT-B2', 'UDDT collection period [d]')</t>
         </is>
       </c>
       <c r="C178" t="inlineStr"/>
@@ -9541,7 +9541,7 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>('UDDT-B2', 'N volatilization [fraction of total N]')</t>
+          <t>('UDDT-B2', 'UDDT N volatilization [fraction of total N]')</t>
         </is>
       </c>
       <c r="C179" t="inlineStr"/>
@@ -9557,7 +9557,7 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>('UDDT-B2', 'Struvite p ksp [-]')</t>
+          <t>('UDDT-B2', 'UDDT struvite p ksp [-]')</t>
         </is>
       </c>
       <c r="C180" t="inlineStr"/>
@@ -9573,7 +9573,7 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>('UDDT-B2', 'Prep sludge [fraction of total precipitate appearing as sludge that settles and can be removed]')</t>
+          <t>('UDDT-B2', 'UDDT prep sludge [fraction of total precipitate appearing as sludge that settles and can be removed]')</t>
         </is>
       </c>
       <c r="C181" t="inlineStr"/>
@@ -9589,7 +9589,7 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>('UDDT-B2', 'Log removal [log unit]')</t>
+          <t>('UDDT-B2', 'UDDT log removal [log unit]')</t>
         </is>
       </c>
       <c r="C182" t="inlineStr"/>
@@ -9605,7 +9605,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>('UDDT-B2', 'Ur p H [pH unit]')</t>
+          <t>('UDDT-B2', 'UDDT ur p H [pH unit]')</t>
         </is>
       </c>
       <c r="C183" t="inlineStr"/>
@@ -9621,7 +9621,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>('UDDT-B2', 'MCF decay [fraction of anaerobic conversion of degraded COD]')</t>
+          <t>('UDDT-B2', 'UDDT MCF decay [fraction of anaerobic conversion of degraded COD]')</t>
         </is>
       </c>
       <c r="C184" t="inlineStr"/>
@@ -9637,7 +9637,7 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>('UDDT-B2', 'N2O EF decay [fraction of N emitted as N2O]')</t>
+          <t>('UDDT-B2', 'UDDT n2o EF decay [fraction of N emitted as N2O]')</t>
         </is>
       </c>
       <c r="C185" t="inlineStr"/>
@@ -9653,7 +9653,7 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>('UDDT-B2', 'Fec moi min [fraction]')</t>
+          <t>('UDDT-B2', 'UDDT fec moi min [fraction]')</t>
         </is>
       </c>
       <c r="C186" t="inlineStr"/>
@@ -9669,7 +9669,7 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>('UDDT-B2', 'Fec moi red rate [1/d]')</t>
+          <t>('UDDT-B2', 'UDDT fec moi red rate [1/d]')</t>
         </is>
       </c>
       <c r="C187" t="inlineStr"/>
@@ -9877,7 +9877,7 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>('Struvite precipitation-B5', 'Material P pipe [m]')</t>
+          <t>('Struvite precipitation-B5', 'Struvite precipitation material P pipe [m]')</t>
         </is>
       </c>
       <c r="C200" t="inlineStr"/>
@@ -9893,7 +9893,7 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>('Struvite precipitation-B5', 'Cost P reactor [USD]')</t>
+          <t>('Struvite precipitation-B5', 'Struvite precipitation cost P reactor [USD]')</t>
         </is>
       </c>
       <c r="C201" t="inlineStr"/>
@@ -9909,7 +9909,7 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>('Struvite precipitation-B5', 'Cost P stirrer [USD/m2]')</t>
+          <t>('Struvite precipitation-B5', 'Struvite precipitation cost P stirrer [USD/m2]')</t>
         </is>
       </c>
       <c r="C202" t="inlineStr"/>
@@ -9925,7 +9925,7 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>('Struvite precipitation-B5', 'Cost P pipe [USD/m]')</t>
+          <t>('Struvite precipitation-B5', 'Struvite precipitation cost P pipe [USD/m]')</t>
         </is>
       </c>
       <c r="C203" t="inlineStr"/>
@@ -9941,7 +9941,7 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>('Struvite precipitation-B5', 'Filter reuse [# times reused]')</t>
+          <t>('Struvite precipitation-B5', 'Struvite precipitation filter reuse [# times reused]')</t>
         </is>
       </c>
       <c r="C204" t="inlineStr"/>
@@ -9957,7 +9957,7 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>('Struvite precipitation-B5', 'Reactor weight [kg]')</t>
+          <t>('Struvite precipitation-B5', 'Struvite precipitation reactor weight [kg]')</t>
         </is>
       </c>
       <c r="C205" t="inlineStr"/>
@@ -9973,7 +9973,7 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>('Struvite precipitation-B5', 'Pvc mass [kg PVC/m]')</t>
+          <t>('Struvite precipitation-B5', 'Struvite precipitation pvc mass [kg PVC/m]')</t>
         </is>
       </c>
       <c r="C206" t="inlineStr"/>
@@ -9989,7 +9989,7 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>('Ion Exchange NH3-B6', 'N rec [%]')</t>
+          <t>('Ion Exchange NH3-B6', 'Ion exchange nh3 N rec [%]')</t>
         </is>
       </c>
       <c r="C207" t="inlineStr"/>
@@ -10005,7 +10005,7 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>('Ion Exchange NH3-B6', 'Resin mass column [g per column]')</t>
+          <t>('Ion Exchange NH3-B6', 'Ion exchange nh3 resin mass column [g per column]')</t>
         </is>
       </c>
       <c r="C208" t="inlineStr"/>
@@ -10021,7 +10021,7 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>('Ion Exchange NH3-B6', 'Material tubing [m]')</t>
+          <t>('Ion Exchange NH3-B6', 'Ion exchange nh3 material tubing [m]')</t>
         </is>
       </c>
       <c r="C209" t="inlineStr"/>
@@ -10037,7 +10037,7 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>('Ion Exchange NH3-B6', 'Cost PVC column [USD/m]')</t>
+          <t>('Ion Exchange NH3-B6', 'Ion exchange nh3 cost PVC column [USD/m]')</t>
         </is>
       </c>
       <c r="C210" t="inlineStr"/>
@@ -10053,7 +10053,7 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>('Ion Exchange NH3-B6', 'Cost tubing [USD/m]')</t>
+          <t>('Ion Exchange NH3-B6', 'Ion exchange nh3 cost tubing [USD/m]')</t>
         </is>
       </c>
       <c r="C211" t="inlineStr"/>
@@ -10069,7 +10069,7 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>('Ion Exchange NH3-B6', 'Cost H2SO4 [USD/metric ton]')</t>
+          <t>('Ion Exchange NH3-B6', 'Ion Exchange NH3 cost H2SO4 [USD/metric ton]')</t>
         </is>
       </c>
       <c r="C212" t="inlineStr"/>
@@ -10085,7 +10085,7 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>('Ion Exchange NH3-B6', 'Cost resin [USD/kg]')</t>
+          <t>('Ion Exchange NH3-B6', 'Ion exchange nh3 cost resin [USD/kg]')</t>
         </is>
       </c>
       <c r="C213" t="inlineStr"/>
@@ -10101,7 +10101,7 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>('Ion Exchange NH3-B6', 'Ad density [mmol N/g resin]')</t>
+          <t>('Ion Exchange NH3-B6', 'Ion exchange nh3 ad density [mmol N/g resin]')</t>
         </is>
       </c>
       <c r="C214" t="inlineStr"/>
@@ -10117,7 +10117,7 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>('Ion Exchange NH3-B6', 'Resin lifetime [cycles]')</t>
+          <t>('Ion Exchange NH3-B6', 'Ion exchange nh3 resin lifetime [cycles]')</t>
         </is>
       </c>
       <c r="C215" t="inlineStr"/>
@@ -10133,7 +10133,7 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>('Ion Exchange NH3-B6', 'Tubing length [m/column]')</t>
+          <t>('Ion Exchange NH3-B6', 'Ion exchange nh3 tubing length [m/column]')</t>
         </is>
       </c>
       <c r="C216" t="inlineStr"/>
@@ -10149,7 +10149,7 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>('Ion Exchange NH3-B6', 'Pvc mass [kg PVC/m]')</t>
+          <t>('Ion Exchange NH3-B6', 'Ion exchange nh3 pvc mass [kg PVC/m]')</t>
         </is>
       </c>
       <c r="C217" t="inlineStr"/>
@@ -10165,7 +10165,7 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>('Ion Exchange NH3-B6', 'Tubing mass [kg PE /m]')</t>
+          <t>('Ion Exchange NH3-B6', 'Ion exchange nh3 tubing mass [kg PE /m]')</t>
         </is>
       </c>
       <c r="C218" t="inlineStr"/>
@@ -10181,7 +10181,7 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>('Ion Exchange NH3-B6', 'Tank mass [kg PE/300 L tank]')</t>
+          <t>('Ion Exchange NH3-B6', 'Ion exchange nh3 tank mass [kg PE/300 L tank]')</t>
         </is>
       </c>
       <c r="C219" t="inlineStr"/>
@@ -10197,7 +10197,7 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>('Ion Exchange NH3-B6', 'Tank cost [USD/tank]')</t>
+          <t>('Ion Exchange NH3-B6', 'Ion exchange nh3 tank cost [USD/tank]')</t>
         </is>
       </c>
       <c r="C220" t="inlineStr"/>
@@ -10213,7 +10213,7 @@
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>('Liquid treatment bed-B7', 'Tau [d]')</t>
+          <t>('Liquid treatment bed-B7', 'Liquid treatment bed tau [d]')</t>
         </is>
       </c>
       <c r="C221" t="inlineStr"/>
@@ -10229,7 +10229,7 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>('Liquid treatment bed-B7', 'COD max decay [% of total COD]')</t>
+          <t>('Liquid treatment bed-B7', 'Liquid treatment bed COD max decay [% of total COD]')</t>
         </is>
       </c>
       <c r="C222" t="inlineStr"/>
@@ -10245,7 +10245,7 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>('Liquid treatment bed-B7', 'MCF decay [% anaerobic conversion of degraded COD]')</t>
+          <t>('Liquid treatment bed-B7', 'Liquid treatment bed MCF decay [% anaerobic conversion of degraded COD]')</t>
         </is>
       </c>
       <c r="C223" t="inlineStr"/>
@@ -10261,7 +10261,7 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>('Liquid treatment bed-B7', 'N max decay [% N removal]')</t>
+          <t>('Liquid treatment bed-B7', 'Liquid treatment bed N max decay [% N removal]')</t>
         </is>
       </c>
       <c r="C224" t="inlineStr"/>
@@ -10277,7 +10277,7 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>('Liquid treatment bed-B7', 'N2O EF decay [% of degraded N emitted as N2O]')</t>
+          <t>('Liquid treatment bed-B7', 'Liquid treatment bed n2o EF decay [% of degraded N emitted as N2O]')</t>
         </is>
       </c>
       <c r="C225" t="inlineStr"/>
@@ -10293,7 +10293,7 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>('Liquid treatment bed-B7', 'Bed H [m]')</t>
+          <t>('Liquid treatment bed-B7', 'Liquid treatment bed bed H [m]')</t>
         </is>
       </c>
       <c r="C226" t="inlineStr"/>
@@ -10309,7 +10309,7 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>('Liquid treatment bed-B7', 'Concrete thickness [m]')</t>
+          <t>('Liquid treatment bed-B7', 'Liquid treatment bed concrete thickness [m]')</t>
         </is>
       </c>
       <c r="C227" t="inlineStr"/>
@@ -10325,7 +10325,7 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>('Control box OP-B8', 'Icp controller board [USD]')</t>
+          <t>('Control box OP-B8', 'Control box OP icp controller board [USD]')</t>
         </is>
       </c>
       <c r="C228" t="inlineStr"/>
@@ -10341,7 +10341,7 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>('Control box OP-B8', 'Icp variable frequence drives [USD]')</t>
+          <t>('Control box OP-B8', 'Control box OP icp variable frequence drives [USD]')</t>
         </is>
       </c>
       <c r="C229" t="inlineStr"/>
@@ -10357,7 +10357,7 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>('Control box OP-B8', 'Icp power meter [USD]')</t>
+          <t>('Control box OP-B8', 'Control box OP icp power meter [USD]')</t>
         </is>
       </c>
       <c r="C230" t="inlineStr"/>
@@ -10373,7 +10373,7 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>('Control box OP-B8', 'Icp line filter [USD]')</t>
+          <t>('Control box OP-B8', 'Control box OP icp line filter [USD]')</t>
         </is>
       </c>
       <c r="C231" t="inlineStr"/>
@@ -10389,7 +10389,7 @@
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>('Control box OP-B8', 'Icp power meter transformer [USD]')</t>
+          <t>('Control box OP-B8', 'Control box OP icp power meter transformer [USD]')</t>
         </is>
       </c>
       <c r="C232" t="inlineStr"/>
@@ -10405,7 +10405,7 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>('Control box OP-B8', 'Icp touch screen [USD]')</t>
+          <t>('Control box OP-B8', 'Control box OP icp touch screen [USD]')</t>
         </is>
       </c>
       <c r="C233" t="inlineStr"/>
@@ -10421,7 +10421,7 @@
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>('Control box OP-B8', 'Electrician replacecables icp [nan]')</t>
+          <t>('Control box OP-B8', 'Control box OP electrician replacecables icp [nan]')</t>
         </is>
       </c>
       <c r="C234" t="inlineStr"/>
@@ -10437,7 +10437,7 @@
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>('Control box OP-B8', 'Electrician replacewires icp [nan]')</t>
+          <t>('Control box OP-B8', 'Control box OP electrician replacewires icp [nan]')</t>
         </is>
       </c>
       <c r="C235" t="inlineStr"/>
@@ -10453,7 +10453,7 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>('Control box OP-B8', 'Service team replacetouchscreen icp [nan]')</t>
+          <t>('Control box OP-B8', 'Control box OP service team replacetouchscreen icp [nan]')</t>
         </is>
       </c>
       <c r="C236" t="inlineStr"/>
@@ -10469,7 +10469,7 @@
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>('Control box OP-B8', 'Facility manager configurevariable icp [nan]')</t>
+          <t>('Control box OP-B8', 'Control box OP facility manager configurevariable icp [nan]')</t>
         </is>
       </c>
       <c r="C237" t="inlineStr"/>
@@ -10485,7 +10485,7 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>('Control box OP-B8', 'Biomass controls replaceboard icp [nan]')</t>
+          <t>('Control box OP-B8', 'Control box OP biomass controls replaceboard icp [nan]')</t>
         </is>
       </c>
       <c r="C238" t="inlineStr"/>
@@ -10501,7 +10501,7 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>('Control box OP-B8', 'Biomass controls codemalfunctioning icp [nan]')</t>
+          <t>('Control box OP-B8', 'Control box OP biomass controls codemalfunctioning icp [nan]')</t>
         </is>
       </c>
       <c r="C239" t="inlineStr"/>
@@ -10517,7 +10517,7 @@
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>('Control box OP-B8', 'Frequency corrective maintenance [y / occurance]')</t>
+          <t>('Control box OP-B8', 'Control box OP frequency corrective maintenance [y / occurance]')</t>
         </is>
       </c>
       <c r="C240" t="inlineStr"/>
@@ -10533,7 +10533,7 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>('Housing biogenic refinery-B9', 'Container20ft cost [USD]')</t>
+          <t>('Housing biogenic refinery-B9', 'Housing biogenic refinery container20ft cost [USD]')</t>
         </is>
       </c>
       <c r="C241" t="inlineStr"/>
@@ -10549,7 +10549,7 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>('Housing biogenic refinery-B9', 'Container40ft cost [USD]')</t>
+          <t>('Housing biogenic refinery-B9', 'Housing biogenic refinery container40ft cost [USD]')</t>
         </is>
       </c>
       <c r="C242" t="inlineStr"/>
@@ -10565,7 +10565,7 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>('Housing biogenic refinery-B9', 'Stainless steel housing [USD per m2]')</t>
+          <t>('Housing biogenic refinery-B9', 'Housing biogenic refinery stainless steel housing [USD per m2]')</t>
         </is>
       </c>
       <c r="C243" t="inlineStr"/>
@@ -10581,7 +10581,7 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>('Housing biogenic refinery-B9', 'Concrete cost [USD per m3]')</t>
+          <t>('Housing biogenic refinery-B9', 'Housing biogenic refinery concrete cost [USD per m3]')</t>
         </is>
       </c>
       <c r="C244" t="inlineStr"/>
@@ -10597,7 +10597,7 @@
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>('Housing biogenic refinery-B9', 'Concrete thickness [m]')</t>
+          <t>('Housing biogenic refinery-B9', 'Housing biogenic refinery concrete thickness [m]')</t>
         </is>
       </c>
       <c r="C245" t="inlineStr"/>
@@ -10613,7 +10613,7 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>('Housing biogenic refinery-B9', 'Footprint [m2]')</t>
+          <t>('Housing biogenic refinery-B9', 'Housing biogenic refinery footprint [m2]')</t>
         </is>
       </c>
       <c r="C246" t="inlineStr"/>

</xml_diff>